<commit_message>
Include state variable results
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="316">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1350,8 +1350,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1392,7 +1392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -1408,12 +1408,11 @@
       <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="str">
-        <f aca="false">IF(F2="",E2,G2)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"account","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegator","type":"address"},{"indexed":true,"internalType":"address","name":"fromDelegate","type":"address"},{"indexed":true,"internalType":"address","name":"toDelegate","type":"address"}],"name":"DelegateChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegate","type":"address"},{"indexed":false,"internalType":"uint256","name":"previousBalance","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newBalance","type":"uint256"}],"name":"DelegateVotesChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"owner","type":"address"},{"indexed":false,"internalType":"address","name":"newOwner","type":"address"}],"name":"OwnerChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DELEGATION_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"DOMAIN_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"abolishSeizing","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_user","type":"address"}],"name":"addToWhitelist","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint32","name":"","type":"uint32"}],"name":"checkpoints","outputs":[{"internalType":"uint32","name":"fromBlock","type":"uint32"},{"internalType":"uint96","name":"votes","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"closeTheGates","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"delegatee","type":"address"}],"name":"delegate","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"delegatee","type":"address"},{"internalType":"uint256","name":"nonce","type":"uint256"},{"internalType":"uint256","name":"expiry","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"delegateBySig","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"delegates","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getCurrentVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"blockNumber","type":"uint256"}],"name":"getPriorVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"mint","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"numCheckpoints","outputs":[{"internalType":"uint32","name":"","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"openTheGates","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_user","type":"address"}],"name":"removeFromWhitelist","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"seizable","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"seize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner_","type":"address"}],"name":"setOwner","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"tradable","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"whitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -1429,12 +1428,11 @@
       <c r="E3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="0" t="str">
-        <f aca="false">IF(F3="",E3,G3)</f>
-        <v>[{"inputs":[{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"minter","type":"address"}],"name":"AddMinter","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"newOperator","type":"address"}],"name":"ChangeOperator","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"minter","type":"address"}],"name":"RemoveMinter","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"minter_","type":"address"}],"name":"addMinter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burn","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"claimOperator","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"mint","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"minters","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"operator","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingOperator","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"minter_","type":"address"}],"name":"removeMinter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newOperator_","type":"address"}],"name":"setPendingOperator","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>17</v>
       </c>
@@ -1450,12 +1448,11 @@
       <c r="E4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="0" t="str">
-        <f aca="false">IF(F4="",E4,G4)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"_singleton","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"stateMutability":"payable","type":"fallback"}]</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
@@ -1471,12 +1468,11 @@
       <c r="E5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="0" t="str">
-        <f aca="false">IF(F5="",E5,G5)</f>
-        <v>[{"inputs":[{"internalType":"contract CErc20","name":"ctoken_","type":"address"},{"internalType":"address","name":"gov_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"constant":true,"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newGov_","type":"address"}],"name":"changeGov","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"contraction","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"ctoken","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"expansion","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"gov","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"resign","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"takeProfit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>26</v>
       </c>
@@ -1492,12 +1488,11 @@
       <c r="E6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="0" t="str">
-        <f aca="false">IF(F6="",E6,G6)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingImplementation","type":"address"}],"name":"NewPendingImplementation","type":"event"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_acceptImplementation","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPendingImplementation","type":"address"}],"name":"_setPendingImplementation","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingComptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
@@ -1513,12 +1508,11 @@
       <c r="E7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="0" t="str">
-        <f aca="false">IF(F7="",E7,G7)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"addAmount","type":"uint256"}],"name":"_addReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>35</v>
       </c>
@@ -1534,12 +1528,11 @@
       <c r="E8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="0" t="str">
-        <f aca="false">IF(F8="",E8,G8)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"addAmount","type":"uint256"}],"name":"_addReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>38</v>
       </c>
@@ -1555,12 +1548,11 @@
       <c r="E9" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="0" t="str">
-        <f aca="false">IF(F9="",E9,G9)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"addAmount","type":"uint256"}],"name":"_addReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>41</v>
       </c>
@@ -1576,12 +1568,11 @@
       <c r="E10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="0" t="str">
-        <f aca="false">IF(F10="",E10,G10)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"},{"internalType":"contract IDelegateRegistry","name":"delegateRegistry_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"addAmount","type":"uint256"}],"name":"_addReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"delegate_","type":"address"}],"name":"delegate","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"delegateRegistry","outputs":[{"internalType":"contract IDelegateRegistry","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>45</v>
       </c>
@@ -1597,12 +1588,11 @@
       <c r="E11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="0" t="str">
-        <f aca="false">IF(F11="",E11,G11)</f>
-        <v>[{"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"contract CToken","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[],"name":"mint","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"repayBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"}],"name":"repayBorrowBehalf","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>49</v>
       </c>
@@ -1618,12 +1608,11 @@
       <c r="E12" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="0" t="str">
-        <f aca="false">IF(F12="",E12,G12)</f>
-        <v>[{"inputs":[{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"minter","type":"address"}],"name":"AddMinter","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"newOperator","type":"address"}],"name":"ChangeOperator","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"minter","type":"address"}],"name":"RemoveMinter","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"minter_","type":"address"}],"name":"addMinter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"burn","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"claimOperator","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"mint","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"minters","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"operator","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingOperator","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"minter_","type":"address"}],"name":"removeMinter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newOperator_","type":"address"}],"name":"setPendingOperator","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>52</v>
       </c>
@@ -1639,12 +1628,11 @@
       <c r="E13" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="0" t="str">
-        <f aca="false">IF(F13="",E13,G13)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>56</v>
       </c>
@@ -1660,12 +1648,11 @@
       <c r="E14" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="0" t="str">
-        <f aca="false">IF(F14="",E14,G14)</f>
-        <v>[{"name":"Transfer","inputs":[{"name":"sender","type":"address","indexed":true},{"name":"receiver","type":"address","indexed":true},{"name":"value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"Approval","inputs":[{"name":"owner","type":"address","indexed":true},{"name":"spender","type":"address","indexed":true},{"name":"value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"TokenExchange","inputs":[{"name":"buyer","type":"address","indexed":true},{"name":"sold_id","type":"int128","indexed":false},{"name":"tokens_sold","type":"uint256","indexed":false},{"name":"bought_id","type":"int128","indexed":false},{"name":"tokens_bought","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"TokenExchangeUnderlying","inputs":[{"name":"buyer","type":"address","indexed":true},{"name":"sold_id","type":"int128","indexed":false},{"name":"tokens_sold","type":"uint256","indexed":false},{"name":"bought_id","type":"int128","indexed":false},{"name":"tokens_bought","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"AddLiquidity","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amounts","type":"uint256[2]","indexed":false},{"name":"fees","type":"uint256[2]","indexed":false},{"name":"invariant","type":"uint256","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RemoveLiquidity","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amounts","type":"uint256[2]","indexed":false},{"name":"fees","type":"uint256[2]","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RemoveLiquidityOne","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amount","type":"uint256","indexed":false},{"name":"coin_amount","type":"uint256","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RemoveLiquidityImbalance","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amounts","type":"uint256[2]","indexed":false},{"name":"fees","type":"uint256[2]","indexed":false},{"name":"invariant","type":"uint256","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RampA","inputs":[{"name":"old_A","type":"uint256","indexed":false},{"name":"new_A","type":"uint256","indexed":false},{"name":"initial_time","type":"uint256","indexed":false},{"name":"future_time","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"StopRampA","inputs":[{"name":"A","type":"uint256","indexed":false},{"name":"t","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"stateMutability":"nonpayable","type":"constructor","inputs":[],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"initialize","inputs":[{"name":"_name","type":"string"},{"name":"_symbol","type":"string"},{"name":"_coin","type":"address"},{"name":"_rate_multiplier","type":"uint256"},{"name":"_A","type":"uint256"},{"name":"_fee","type":"uint256"}],"outputs":[],"gas":450772},{"stateMutability":"view","type":"function","name":"decimals","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":318},{"stateMutability":"nonpayable","type":"function","name":"transfer","inputs":[{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":77977},{"stateMutability":"nonpayable","type":"function","name":"transferFrom","inputs":[{"name":"_from","type":"address"},{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":115912},{"stateMutability":"nonpayable","type":"function","name":"approve","inputs":[{"name":"_spender","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":37851},{"stateMutability":"view","type":"function","name":"admin_fee","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":438},{"stateMutability":"view","type":"function","name":"A","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":10704},{"stateMutability":"view","type":"function","name":"A_precise","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":10666},{"stateMutability":"view","type":"function","name":"get_virtual_price","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":1023280},{"stateMutability":"view","type":"function","name":"calc_token_amount","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_is_deposit","type":"bool"}],"outputs":[{"name":"","type":"uint256"}],"gas":4029742},{"stateMutability":"nonpayable","type":"function","name":"add_liquidity","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_min_mint_amount","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"add_liquidity","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_min_mint_amount","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"view","type":"function","name":"get_dy","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"dx","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":2466478},{"stateMutability":"view","type":"function","name":"get_dy_underlying","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"dx","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":2475029},{"stateMutability":"nonpayable","type":"function","name":"exchange","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"exchange","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"exchange_underlying","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"exchange_underlying","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"_min_amounts","type":"uint256[2]"}],"outputs":[{"name":"","type":"uint256[2]"}]},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"_min_amounts","type":"uint256[2]"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256[2]"}]},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_imbalance","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_max_burn_amount","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_imbalance","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_max_burn_amount","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"view","type":"function","name":"calc_withdraw_one_coin","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"i","type":"int128"}],"outputs":[{"name":"","type":"uint256"}],"gas":1130},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_one_coin","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"i","type":"int128"},{"name":"_min_received","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_one_coin","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"i","type":"int128"},{"name":"_min_received","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}]},{"stateMutability":"nonpayable","type":"function","name":"ramp_A","inputs":[{"name":"_future_A","type":"uint256"},{"name":"_future_time","type":"uint256"}],"outputs":[],"gas":162101},{"stateMutability":"nonpayable","type":"function","name":"stop_ramp_A","inputs":[],"outputs":[],"gas":157565},{"stateMutability":"view","type":"function","name":"admin_balances","inputs":[{"name":"i","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":7770},{"stateMutability":"nonpayable","type":"function","name":"withdraw_admin_fees","inputs":[],"outputs":[],"gas":40657},{"stateMutability":"view","type":"function","name":"coins","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"address"}],"gas":3123},{"stateMutability":"view","type":"function","name":"balances","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":3153},{"stateMutability":"view","type":"function","name":"fee","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3138},{"stateMutability":"view","type":"function","name":"initial_A","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3168},{"stateMutability":"view","type":"function","name":"future_A","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3198},{"stateMutability":"view","type":"function","name":"initial_A_time","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3228},{"stateMutability":"view","type":"function","name":"future_A_time","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3258},{"stateMutability":"view","type":"function","name":"name","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":13518},{"stateMutability":"view","type":"function","name":"symbol","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":11271},{"stateMutability":"view","type":"function","name":"balanceOf","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3563},{"stateMutability":"view","type":"function","name":"allowance","inputs":[{"name":"arg0","type":"address"},{"name":"arg1","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3808},{"stateMutability":"view","type":"function","name":"totalSupply","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3408}]</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>61</v>
       </c>
@@ -1681,12 +1668,11 @@
       <c r="E15" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="0" t="str">
-        <f aca="false">IF(F15="",E15,G15)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"_operator","type":"address"},{"internalType":"address","name":"_lptoken","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_from","type":"address"},{"internalType":"uint256","name":"_amount","type":"uint256"}],"name":"burn","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"_to","type":"address"},{"internalType":"uint256","name":"_amount","type":"uint256"}],"name":"mint","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"operator","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"sender","type":"address"},{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>65</v>
       </c>
@@ -1708,12 +1694,11 @@
       <c r="G16" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="0" t="str">
-        <f aca="false">IF(F16="",E16,G16)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>71</v>
       </c>
@@ -1735,12 +1720,11 @@
       <c r="G17" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="0" t="str">
-        <f aca="false">IF(F17="",E17,G17)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>74</v>
       </c>
@@ -1762,12 +1746,11 @@
       <c r="G18" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="0" t="str">
-        <f aca="false">IF(F18="",E18,G18)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>78</v>
       </c>
@@ -1789,12 +1772,11 @@
       <c r="G19" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="0" t="str">
-        <f aca="false">IF(F19="",E19,G19)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>81</v>
       </c>
@@ -1816,12 +1798,11 @@
       <c r="G20" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="0" t="str">
-        <f aca="false">IF(F20="",E20,G20)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>84</v>
       </c>
@@ -1843,12 +1824,11 @@
       <c r="G21" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="0" t="str">
-        <f aca="false">IF(F21="",E21,G21)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>87</v>
       </c>
@@ -1870,12 +1850,11 @@
       <c r="G22" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="0" t="str">
-        <f aca="false">IF(F22="",E22,G22)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>90</v>
       </c>
@@ -1897,12 +1876,11 @@
       <c r="G23" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="0" t="str">
-        <f aca="false">IF(F23="",E23,G23)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>93</v>
       </c>
@@ -1924,12 +1902,11 @@
       <c r="G24" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="0" t="str">
-        <f aca="false">IF(F24="",E24,G24)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>96</v>
       </c>
@@ -1951,12 +1928,11 @@
       <c r="G25" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H25" s="0" t="str">
-        <f aca="false">IF(F25="",E25,G25)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>99</v>
       </c>
@@ -1978,12 +1954,11 @@
       <c r="G26" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="0" t="str">
-        <f aca="false">IF(F26="",E26,G26)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>103</v>
       </c>
@@ -2005,12 +1980,11 @@
       <c r="G27" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="0" t="str">
-        <f aca="false">IF(F27="",E27,G27)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H27" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>107</v>
       </c>
@@ -2032,12 +2006,11 @@
       <c r="G28" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="0" t="str">
-        <f aca="false">IF(F28="",E28,G28)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>110</v>
       </c>
@@ -2059,12 +2032,11 @@
       <c r="G29" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H29" s="0" t="str">
-        <f aca="false">IF(F29="",E29,G29)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H29" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>113</v>
       </c>
@@ -2086,12 +2058,11 @@
       <c r="G30" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H30" s="0" t="str">
-        <f aca="false">IF(F30="",E30,G30)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H30" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>116</v>
       </c>
@@ -2113,12 +2084,11 @@
       <c r="G31" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="0" t="str">
-        <f aca="false">IF(F31="",E31,G31)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H31" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>119</v>
       </c>
@@ -2140,12 +2110,11 @@
       <c r="G32" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H32" s="0" t="str">
-        <f aca="false">IF(F32="",E32,G32)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H32" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>122</v>
       </c>
@@ -2167,12 +2136,11 @@
       <c r="G33" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="0" t="str">
-        <f aca="false">IF(F33="",E33,G33)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H33" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>125</v>
       </c>
@@ -2194,12 +2162,11 @@
       <c r="G34" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="0" t="str">
-        <f aca="false">IF(F34="",E34,G34)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H34" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>128</v>
       </c>
@@ -2221,12 +2188,11 @@
       <c r="G35" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H35" s="0" t="str">
-        <f aca="false">IF(F35="",E35,G35)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>131</v>
       </c>
@@ -2248,12 +2214,11 @@
       <c r="G36" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="0" t="str">
-        <f aca="false">IF(F36="",E36,G36)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>134</v>
       </c>
@@ -2275,12 +2240,11 @@
       <c r="G37" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H37" s="0" t="str">
-        <f aca="false">IF(F37="",E37,G37)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>137</v>
       </c>
@@ -2296,12 +2260,11 @@
       <c r="E38" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="H38" s="0" t="str">
-        <f aca="false">IF(F38="",E38,G38)</f>
-        <v>[{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"inputs":[],"name":"DST_DOLA","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"DST_MARKET","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"GOV","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"SRC_BRIDGE","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"SRC_DOLA","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstBoard","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"dstContraction","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"dstExpansion","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstIsChairSuspended","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"dstLastSuspendTimestamp","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"dstSendProfitToGov","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newBoard","type":"address"}],"name":"dstSetBoard","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"dstSuspendChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"dstTransferReservesToSrc","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstUnsuspendChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"srcBurnReserves","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"srcMintReserves","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"srcTransferReservesToDst","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"contract ERC20","name":"token","type":"address"},{"internalType":"address","name":"to","type":"address"}],"name":"sweep","outputs":[],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>141</v>
       </c>
@@ -2317,12 +2280,11 @@
       <c r="E39" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="H39" s="0" t="str">
-        <f aca="false">IF(F39="",E39,G39)</f>
-        <v>[{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"inputs":[],"name":"DST_DOLA","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"DST_MARKET","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"GOV","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"SRC_BRIDGE","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"SRC_DOLA","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstBoard","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"dstContraction","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"dstExpansion","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstIsChairSuspended","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"dstLastSuspendTimestamp","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"dstSendProfitToGov","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newBoard","type":"address"}],"name":"dstSetBoard","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"dstSuspendChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"dstTransferReservesToSrc","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"dstUnsuspendChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"srcBurnReserves","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"srcMintReserves","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"srcTransferReservesToDst","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"contract ERC20","name":"token","type":"address"},{"internalType":"address","name":"to","type":"address"}],"name":"sweep","outputs":[],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>142</v>
       </c>
@@ -2344,12 +2306,11 @@
       <c r="G40" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H40" s="0" t="str">
-        <f aca="false">IF(F40="",E40,G40)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>145</v>
       </c>
@@ -2371,12 +2332,11 @@
       <c r="G41" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H41" s="0" t="str">
-        <f aca="false">IF(F41="",E41,G41)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>148</v>
       </c>
@@ -2398,12 +2358,11 @@
       <c r="G42" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H42" s="0" t="str">
-        <f aca="false">IF(F42="",E42,G42)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>151</v>
       </c>
@@ -2425,12 +2384,11 @@
       <c r="G43" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H43" s="0" t="str">
-        <f aca="false">IF(F43="",E43,G43)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>154</v>
       </c>
@@ -2446,12 +2404,11 @@
       <c r="E44" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H44" s="0" t="str">
-        <f aca="false">IF(F44="",E44,G44)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>156</v>
       </c>
@@ -2473,12 +2430,11 @@
       <c r="G45" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H45" s="0" t="str">
-        <f aca="false">IF(F45="",E45,G45)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>160</v>
       </c>
@@ -2500,12 +2456,11 @@
       <c r="G46" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="H46" s="0" t="str">
-        <f aca="false">IF(F46="",E46,G46)</f>
-        <v>[{"anonymous":false,"inputs":[{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"rewardsDistributor","type":"address"}],"name":"AddedRewardsDistributor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enabled","type":"bool"}],"name":"AutoImplementationsToggled","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketEntered","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketExited","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketListed","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketUnlisted","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newBorrowCap","type":"uint256"}],"name":"NewBorrowCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldBorrowCapGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"NewBorrowCapGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldCloseFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"NewCloseFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"oldCollateralFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"NewCollateralFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldLiquidationIncentiveMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"NewLiquidationIncentive","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPauseGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"NewPauseGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract PriceOracle","name":"oldPriceOracle","type":"address"},{"indexed":false,"internalType":"contract PriceOracle","name":"newPriceOracle","type":"address"}],"name":"NewPriceOracle","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newSupplyCap","type":"uint256"}],"name":"NewSupplyCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enforce","type":"bool"}],"name":"WhitelistEnforcementChanged","type":"event"},{"constant":false,"inputs":[{"internalType":"address","name":"distributor","type":"address"}],"name":"_addRewardsDistributor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_afterNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract Unitroller","name":"unitroller","type":"address"}],"name":"_become","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_beforeNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"isCEther","type":"bool"},{"internalType":"bytes","name":"constructorData","type":"bytes"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"name":"_deployMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"_setBorrowCapGuardian","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setBorrowPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"_setCloseFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"_setCollateralFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"_setLiquidationIncentive","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newBorrowCaps","type":"uint256[]"}],"name":"_setMarketBorrowCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newSupplyCaps","type":"uint256[]"}],"name":"_setMarketSupplyCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setMintPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"_setPauseGuardian","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract PriceOracle","name":"newOracle","type":"address"}],"name":"_setPriceOracle","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setSeizePaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setTransferPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enforce","type":"bool"}],"name":"_setWhitelistEnforcement","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"suppliers","type":"address[]"},{"internalType":"bool[]","name":"statuses","type":"bool[]"}],"name":"_setWhitelistStatuses","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enabled","type":"bool"}],"name":"_toggleAutoImplementations","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"_unsupportMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint256","name":"","type":"uint256"}],"name":"accountAssets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"adminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allBorrowers","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allMarkets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"autoImplementation","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowCapGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"accountBorrowsNew","type":"uint256"}],"name":"borrowWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"cTokensByUnderlying","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"checkMembership","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"closeFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"enforceWhitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"cTokens","type":"address[]"}],"name":"enterMarkets","outputs":[{"internalType":"uint256[]","name":"","type":"uint256[]"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenAddress","type":"address"}],"name":"exitMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"fuseAdminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllBorrowers","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllMarkets","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAssetsIn","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"address","name":"cTokenModify","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"getHypotheticalAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getRewardsDistributors","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getWhitelist","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isComptroller","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"isDeprecated","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"liquidateBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"liquidateBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"}],"name":"liquidateCalculateSeizeTokens","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"liquidationIncentiveMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"markets","outputs":[{"internalType":"bool","name":"isListed","type":"bool"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"actualMintAmount","type":"uint256"},{"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"mintVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"exchangeRateMantissa","type":"uint256"},{"internalType":"uint256","name":"accountTokens","type":"uint256"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"oracle","outputs":[{"internalType":"contract PriceOracle","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pauseGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingComptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"borrowerIndex","type":"uint256"}],"name":"repayBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"rewardsDistributors","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"seizeGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"suppliers","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"supplyCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"transferGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"whitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"whitelistArray","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>164</v>
       </c>
@@ -2527,12 +2482,11 @@
       <c r="G47" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="H47" s="0" t="str">
-        <f aca="false">IF(F47="",E47,G47)</f>
-        <v>[{"anonymous":false,"inputs":[{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"rewardsDistributor","type":"address"}],"name":"AddedRewardsDistributor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enabled","type":"bool"}],"name":"AutoImplementationsToggled","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketEntered","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketExited","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketListed","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketUnlisted","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newBorrowCap","type":"uint256"}],"name":"NewBorrowCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldBorrowCapGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"NewBorrowCapGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldCloseFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"NewCloseFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"oldCollateralFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"NewCollateralFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldLiquidationIncentiveMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"NewLiquidationIncentive","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPauseGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"NewPauseGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract PriceOracle","name":"oldPriceOracle","type":"address"},{"indexed":false,"internalType":"contract PriceOracle","name":"newPriceOracle","type":"address"}],"name":"NewPriceOracle","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newSupplyCap","type":"uint256"}],"name":"NewSupplyCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enforce","type":"bool"}],"name":"WhitelistEnforcementChanged","type":"event"},{"constant":false,"inputs":[{"internalType":"address","name":"distributor","type":"address"}],"name":"_addRewardsDistributor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_afterNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract Unitroller","name":"unitroller","type":"address"}],"name":"_become","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_beforeNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"isCEther","type":"bool"},{"internalType":"bytes","name":"constructorData","type":"bytes"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"name":"_deployMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"_setBorrowCapGuardian","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setBorrowPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"_setCloseFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"_setCollateralFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"_setLiquidationIncentive","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newBorrowCaps","type":"uint256[]"}],"name":"_setMarketBorrowCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newSupplyCaps","type":"uint256[]"}],"name":"_setMarketSupplyCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setMintPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"_setPauseGuardian","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract PriceOracle","name":"newOracle","type":"address"}],"name":"_setPriceOracle","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setSeizePaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setTransferPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enforce","type":"bool"}],"name":"_setWhitelistEnforcement","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"suppliers","type":"address[]"},{"internalType":"bool[]","name":"statuses","type":"bool[]"}],"name":"_setWhitelistStatuses","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enabled","type":"bool"}],"name":"_toggleAutoImplementations","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"_unsupportMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint256","name":"","type":"uint256"}],"name":"accountAssets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"adminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allBorrowers","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allMarkets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"autoImplementation","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowCapGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"accountBorrowsNew","type":"uint256"}],"name":"borrowWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"cTokensByUnderlying","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"checkMembership","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"closeFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"enforceWhitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"cTokens","type":"address[]"}],"name":"enterMarkets","outputs":[{"internalType":"uint256[]","name":"","type":"uint256[]"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenAddress","type":"address"}],"name":"exitMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"fuseAdminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllBorrowers","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllMarkets","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAssetsIn","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"address","name":"cTokenModify","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"getHypotheticalAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getRewardsDistributors","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getWhitelist","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isComptroller","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"isDeprecated","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"liquidateBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"liquidateBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"}],"name":"liquidateCalculateSeizeTokens","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"liquidationIncentiveMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"markets","outputs":[{"internalType":"bool","name":"isListed","type":"bool"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"actualMintAmount","type":"uint256"},{"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"mintVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"exchangeRateMantissa","type":"uint256"},{"internalType":"uint256","name":"accountTokens","type":"uint256"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"oracle","outputs":[{"internalType":"contract PriceOracle","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pauseGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingComptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"borrowerIndex","type":"uint256"}],"name":"repayBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"rewardsDistributors","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"seizeGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"suppliers","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"supplyCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"transferGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"whitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"whitelistArray","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>168</v>
       </c>
@@ -2554,12 +2508,11 @@
       <c r="G48" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="H48" s="0" t="str">
-        <f aca="false">IF(F48="",E48,G48)</f>
-        <v>[{"anonymous":false,"inputs":[{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"rewardsDistributor","type":"address"}],"name":"AddedRewardsDistributor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enabled","type":"bool"}],"name":"AutoImplementationsToggled","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketEntered","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketExited","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketListed","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketUnlisted","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newBorrowCap","type":"uint256"}],"name":"NewBorrowCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldBorrowCapGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"NewBorrowCapGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldCloseFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"NewCloseFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"oldCollateralFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"NewCollateralFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldLiquidationIncentiveMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"NewLiquidationIncentive","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPauseGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"NewPauseGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract PriceOracle","name":"oldPriceOracle","type":"address"},{"indexed":false,"internalType":"contract PriceOracle","name":"newPriceOracle","type":"address"}],"name":"NewPriceOracle","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newSupplyCap","type":"uint256"}],"name":"NewSupplyCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enforce","type":"bool"}],"name":"WhitelistEnforcementChanged","type":"event"},{"constant":false,"inputs":[{"internalType":"address","name":"distributor","type":"address"}],"name":"_addRewardsDistributor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_afterNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract Unitroller","name":"unitroller","type":"address"}],"name":"_become","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_beforeNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"isCEther","type":"bool"},{"internalType":"bytes","name":"constructorData","type":"bytes"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"name":"_deployMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"_setBorrowCapGuardian","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setBorrowPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"_setCloseFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"_setCollateralFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"_setLiquidationIncentive","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newBorrowCaps","type":"uint256[]"}],"name":"_setMarketBorrowCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newSupplyCaps","type":"uint256[]"}],"name":"_setMarketSupplyCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setMintPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"_setPauseGuardian","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract PriceOracle","name":"newOracle","type":"address"}],"name":"_setPriceOracle","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setSeizePaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setTransferPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enforce","type":"bool"}],"name":"_setWhitelistEnforcement","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"suppliers","type":"address[]"},{"internalType":"bool[]","name":"statuses","type":"bool[]"}],"name":"_setWhitelistStatuses","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enabled","type":"bool"}],"name":"_toggleAutoImplementations","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"_unsupportMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint256","name":"","type":"uint256"}],"name":"accountAssets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"adminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allBorrowers","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allMarkets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"autoImplementation","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowCapGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"accountBorrowsNew","type":"uint256"}],"name":"borrowWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"cTokensByUnderlying","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"checkMembership","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"closeFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"enforceWhitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"cTokens","type":"address[]"}],"name":"enterMarkets","outputs":[{"internalType":"uint256[]","name":"","type":"uint256[]"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenAddress","type":"address"}],"name":"exitMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"fuseAdminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllBorrowers","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllMarkets","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAssetsIn","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"address","name":"cTokenModify","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"getHypotheticalAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getRewardsDistributors","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getWhitelist","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isComptroller","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"isDeprecated","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"liquidateBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"liquidateBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"}],"name":"liquidateCalculateSeizeTokens","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"liquidationIncentiveMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"markets","outputs":[{"internalType":"bool","name":"isListed","type":"bool"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"actualMintAmount","type":"uint256"},{"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"mintVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"exchangeRateMantissa","type":"uint256"},{"internalType":"uint256","name":"accountTokens","type":"uint256"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"oracle","outputs":[{"internalType":"contract PriceOracle","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pauseGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingComptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"borrowerIndex","type":"uint256"}],"name":"repayBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"rewardsDistributors","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"seizeGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"suppliers","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"supplyCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"transferGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"whitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"whitelistArray","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>171</v>
       </c>
@@ -2581,12 +2534,11 @@
       <c r="G49" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="H49" s="0" t="str">
-        <f aca="false">IF(F49="",E49,G49)</f>
-        <v>[{"anonymous":false,"inputs":[{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"string","name":"action","type":"string"},{"indexed":false,"internalType":"bool","name":"pauseState","type":"bool"}],"name":"ActionPaused","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"rewardsDistributor","type":"address"}],"name":"AddedRewardsDistributor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enabled","type":"bool"}],"name":"AutoImplementationsToggled","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketEntered","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"address","name":"account","type":"address"}],"name":"MarketExited","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketListed","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"MarketUnlisted","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newBorrowCap","type":"uint256"}],"name":"NewBorrowCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldBorrowCapGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"NewBorrowCapGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldCloseFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"NewCloseFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"oldCollateralFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"NewCollateralFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldLiquidationIncentiveMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"NewLiquidationIncentive","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPauseGuardian","type":"address"},{"indexed":false,"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"NewPauseGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract PriceOracle","name":"oldPriceOracle","type":"address"},{"indexed":false,"internalType":"contract PriceOracle","name":"newPriceOracle","type":"address"}],"name":"NewPriceOracle","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"contract CToken","name":"cToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"newSupplyCap","type":"uint256"}],"name":"NewSupplyCap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"bool","name":"enforce","type":"bool"}],"name":"WhitelistEnforcementChanged","type":"event"},{"constant":false,"inputs":[{"internalType":"address","name":"distributor","type":"address"}],"name":"_addRewardsDistributor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_afterNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract Unitroller","name":"unitroller","type":"address"}],"name":"_become","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_beforeNonReentrant","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"isCEther","type":"bool"},{"internalType":"bytes","name":"constructorData","type":"bytes"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"name":"_deployMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"_mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newBorrowCapGuardian","type":"address"}],"name":"_setBorrowCapGuardian","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setBorrowPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newCloseFactorMantissa","type":"uint256"}],"name":"_setCloseFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"uint256","name":"newCollateralFactorMantissa","type":"uint256"}],"name":"_setCollateralFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newLiquidationIncentiveMantissa","type":"uint256"}],"name":"_setLiquidationIncentive","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newBorrowCaps","type":"uint256[]"}],"name":"_setMarketBorrowCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken[]","name":"cTokens","type":"address[]"},{"internalType":"uint256[]","name":"newSupplyCaps","type":"uint256[]"}],"name":"_setMarketSupplyCaps","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"},{"internalType":"bool","name":"state","type":"bool"}],"name":"_setMintPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPauseGuardian","type":"address"}],"name":"_setPauseGuardian","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract PriceOracle","name":"newOracle","type":"address"}],"name":"_setPriceOracle","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setSeizePaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"state","type":"bool"}],"name":"_setTransferPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enforce","type":"bool"}],"name":"_setWhitelistEnforcement","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"suppliers","type":"address[]"},{"internalType":"bool[]","name":"statuses","type":"bool[]"}],"name":"_setWhitelistStatuses","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"bool","name":"enabled","type":"bool"}],"name":"_toggleAutoImplementations","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"_unsupportMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint256","name":"","type":"uint256"}],"name":"accountAssets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"adminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allBorrowers","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"allMarkets","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"autoImplementation","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowCapGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"borrowGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"accountBorrowsNew","type":"uint256"}],"name":"borrowWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"cTokensByUnderlying","outputs":[{"internalType":"contract CToken","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"checkMembership","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"closeFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"enforceWhitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"cTokens","type":"address[]"}],"name":"enterMarkets","outputs":[{"internalType":"uint256[]","name":"","type":"uint256[]"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenAddress","type":"address"}],"name":"exitMarket","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"fuseAdminHasRights","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllBorrowers","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getAllMarkets","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAssetsIn","outputs":[{"internalType":"contract CToken[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"address","name":"cTokenModify","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"},{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"getHypotheticalAccountLiquidity","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getRewardsDistributors","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getWhitelist","outputs":[{"internalType":"address[]","name":"","type":"address[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isComptroller","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"contract CToken","name":"cToken","type":"address"}],"name":"isDeprecated","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"liquidateBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"liquidateBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"}],"name":"liquidateCalculateSeizeTokens","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"liquidationIncentiveMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"markets","outputs":[{"internalType":"bool","name":"isListed","type":"bool"},{"internalType":"uint256","name":"collateralFactorMantissa","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"mintGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"minter","type":"address"},{"internalType":"uint256","name":"actualMintAmount","type":"uint256"},{"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"mintVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"uint256","name":"exchangeRateMantissa","type":"uint256"},{"internalType":"uint256","name":"accountTokens","type":"uint256"},{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mintWithinLimits","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"oracle","outputs":[{"internalType":"contract PriceOracle","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pauseGuardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingComptrollerImplementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"redeemer","type":"address"},{"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeemVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"payer","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"actualRepayAmount","type":"uint256"},{"internalType":"uint256","name":"borrowerIndex","type":"uint256"}],"name":"repayBorrowVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"rewardsDistributors","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"seizeGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cTokenCollateral","type":"address"},{"internalType":"address","name":"cTokenBorrowed","type":"address"},{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seizeVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"suppliers","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"supplyCaps","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferAllowed","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"transferGuardianPaused","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"cToken","type":"address"},{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"transferTokens","type":"uint256"}],"name":"transferVerify","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"whitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"whitelistArray","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H49" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>174</v>
       </c>
@@ -2602,12 +2554,11 @@
       <c r="E50" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H50" s="0" t="str">
-        <f aca="false">IF(F50="",E50,G50)</f>
-        <v>[{"inputs":[{"internalType":"contract CErc20","name":"ctoken_","type":"address"},{"internalType":"address","name":"gov_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"constant":true,"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newGov_","type":"address"}],"name":"changeGov","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"contraction","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"ctoken","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"expansion","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"gov","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"resign","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"takeProfit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H50" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>177</v>
       </c>
@@ -2623,12 +2574,11 @@
       <c r="E51" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H51" s="0" t="str">
-        <f aca="false">IF(F51="",E51,G51)</f>
-        <v>[{"inputs":[{"internalType":"contract CErc20","name":"ctoken_","type":"address"},{"internalType":"address","name":"gov_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"constant":true,"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newGov_","type":"address"}],"name":"changeGov","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"contraction","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"ctoken","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"expansion","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"gov","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"resign","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"takeProfit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H51" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>180</v>
       </c>
@@ -2644,12 +2594,11 @@
       <c r="E52" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H52" s="0" t="str">
-        <f aca="false">IF(F52="",E52,G52)</f>
-        <v>[{"inputs":[{"internalType":"contract CErc20","name":"ctoken_","type":"address"},{"internalType":"address","name":"gov_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"constant":true,"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newGov_","type":"address"}],"name":"changeGov","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"contraction","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"ctoken","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"expansion","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"gov","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"resign","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"takeProfit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H52" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>183</v>
       </c>
@@ -2665,12 +2614,11 @@
       <c r="E53" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H53" s="0" t="str">
-        <f aca="false">IF(F53="",E53,G53)</f>
-        <v>[{"inputs":[{"internalType":"contract CErc20","name":"ctoken_","type":"address"},{"internalType":"address","name":"gov_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"constant":true,"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newGov_","type":"address"}],"name":"changeGov","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"contraction","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"ctoken","outputs":[{"internalType":"contract CErc20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"expansion","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"gov","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"resign","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"takeProfit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"contract ERC20","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H53" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>186</v>
       </c>
@@ -2692,12 +2640,11 @@
       <c r="G54" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H54" s="0" t="str">
-        <f aca="false">IF(F54="",E54,G54)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H54" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>189</v>
       </c>
@@ -2719,12 +2666,11 @@
       <c r="G55" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H55" s="0" t="str">
-        <f aca="false">IF(F55="",E55,G55)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H55" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>192</v>
       </c>
@@ -2746,12 +2692,11 @@
       <c r="G56" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="H56" s="0" t="str">
-        <f aca="false">IF(F56="",E56,G56)</f>
-        <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldAdminFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"NewAdminFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldFuseFeeMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newFuseFeeMantissa","type":"uint256"}],"name":"NewFuseFee","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"_becomeImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"compLikeDelegatee","type":"address"}],"name":"_delegateCompLikeTo","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"_prepare","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newAdminFeeMantissa","type":"uint256"}],"name":"_setAdminFee","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementationSafe","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"string","name":"_name","type":"string"},{"internalType":"string","name":"_symbol","type":"string"}],"name":"_setNameAndSymbol","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"withdrawAmount","type":"uint256"}],"name":"_withdrawFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"adminFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"fuseFeeMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint256","name":"reserveFactorMantissa_","type":"uint256"},{"internalType":"uint256","name":"adminFeeMantissa_","type":"uint256"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCEther","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"protocolSeizeShareMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalAdminFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalFuseFees","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H56" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>193</v>
       </c>
@@ -2767,12 +2712,11 @@
       <c r="E57" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="H57" s="0" t="str">
-        <f aca="false">IF(F57="",E57,G57)</f>
-        <v>[{"inputs":[{"internalType":"contract TimelockInterface","name":"timelock_","type":"address"},{"internalType":"contract InvInterface","name":"inv_","type":"address"},{"internalType":"contract XinvInterface","name":"xinv_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"guardian","type":"address"}],"name":"NewGuardian","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"id","type":"uint256"}],"name":"ProposalCanceled","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"id","type":"uint256"},{"indexed":false,"internalType":"address","name":"proposer","type":"address"},{"indexed":false,"internalType":"address[]","name":"targets","type":"address[]"},{"indexed":false,"internalType":"uint256[]","name":"values","type":"uint256[]"},{"indexed":false,"internalType":"string[]","name":"signatures","type":"string[]"},{"indexed":false,"internalType":"bytes[]","name":"calldatas","type":"bytes[]"},{"indexed":false,"internalType":"uint256","name":"startBlock","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"endBlock","type":"uint256"},{"indexed":false,"internalType":"string","name":"description","type":"string"}],"name":"ProposalCreated","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"id","type":"uint256"}],"name":"ProposalExecuted","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"id","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"eta","type":"uint256"}],"name":"ProposalQueued","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldThreshold","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newThreshold","type":"uint256"}],"name":"ProposalThresholdUpdated","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"proposer","type":"address"},{"indexed":false,"internalType":"bool","name":"value","type":"bool"}],"name":"ProposerWhitelistUpdated","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldQuorum","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newQuorum","type":"uint256"}],"name":"QuorumUpdated","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"voter","type":"address"},{"indexed":false,"internalType":"uint256","name":"proposalId","type":"uint256"},{"indexed":false,"internalType":"bool","name":"support","type":"bool"},{"indexed":false,"internalType":"uint256","name":"votes","type":"uint256"}],"name":"VoteCast","type":"event"},{"constant":true,"inputs":[],"name":"BALLOT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"DOMAIN_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPendingAdmin","type":"address"},{"internalType":"uint256","name":"eta","type":"uint256"}],"name":"__executeSetTimelockPendingAdmin","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newPendingAdmin","type":"address"},{"internalType":"uint256","name":"eta","type":"uint256"}],"name":"__queueSetTimelockPendingAdmin","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"acceptAdmin","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"}],"name":"cancel","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"},{"internalType":"bool","name":"support","type":"bool"}],"name":"castVote","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"},{"internalType":"bool","name":"support","type":"bool"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"castVoteBySig","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"}],"name":"execute","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"}],"name":"getActions","outputs":[{"internalType":"address[]","name":"targets","type":"address[]"},{"internalType":"uint256[]","name":"values","type":"uint256[]"},{"internalType":"string[]","name":"signatures","type":"string[]"},{"internalType":"bytes[]","name":"calldatas","type":"bytes[]"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"},{"internalType":"address","name":"voter","type":"address"}],"name":"getReceipt","outputs":[{"components":[{"internalType":"bool","name":"hasVoted","type":"bool"},{"internalType":"bool","name":"support","type":"bool"},{"internalType":"uint96","name":"votes","type":"uint96"}],"internalType":"struct GovernorMills.Receipt","name":"","type":"tuple"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"guardian","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"inv","outputs":[{"internalType":"contract InvInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"latestProposalIds","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"proposalCount","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"proposalMaxOperations","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"pure","type":"function"},{"constant":true,"inputs":[],"name":"proposalThreshold","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"proposals","outputs":[{"internalType":"uint256","name":"id","type":"uint256"},{"internalType":"address","name":"proposer","type":"address"},{"internalType":"uint256","name":"eta","type":"uint256"},{"internalType":"uint256","name":"startBlock","type":"uint256"},{"internalType":"uint256","name":"endBlock","type":"uint256"},{"internalType":"uint256","name":"forVotes","type":"uint256"},{"internalType":"uint256","name":"againstVotes","type":"uint256"},{"internalType":"bool","name":"canceled","type":"bool"},{"internalType":"bool","name":"executed","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address[]","name":"targets","type":"address[]"},{"internalType":"uint256[]","name":"values","type":"uint256[]"},{"internalType":"string[]","name":"signatures","type":"string[]"},{"internalType":"bytes[]","name":"calldatas","type":"bytes[]"},{"internalType":"string","name":"description","type":"string"}],"name":"propose","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"proposerWhitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"}],"name":"queue","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"quorumVotes","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_newGuardian","type":"address"}],"name":"setGuardian","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"proposalId","type":"uint256"}],"name":"state","outputs":[{"internalType":"enum GovernorMills.ProposalState","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"timelock","outputs":[{"internalType":"contract TimelockInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newQuorum","type":"uint256"}],"name":"updateProposalQuorum","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newThreshold","type":"uint256"}],"name":"updateProposalThreshold","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"proposer","type":"address"},{"internalType":"bool","name":"value","type":"bool"}],"name":"updateProposerWhitelist","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"votingDelay","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"pure","type":"function"},{"constant":true,"inputs":[],"name":"votingPeriod","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"pure","type":"function"},{"constant":true,"inputs":[],"name":"xinv","outputs":[{"internalType":"contract XinvInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"xinvExchangeRates","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H57" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>198</v>
       </c>
@@ -2788,12 +2732,11 @@
       <c r="E58" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="0" t="str">
-        <f aca="false">IF(F58="",E58,G58)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"account","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegator","type":"address"},{"indexed":true,"internalType":"address","name":"fromDelegate","type":"address"},{"indexed":true,"internalType":"address","name":"toDelegate","type":"address"}],"name":"DelegateChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegate","type":"address"},{"indexed":false,"internalType":"uint256","name":"previousBalance","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newBalance","type":"uint256"}],"name":"DelegateVotesChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"owner","type":"address"},{"indexed":false,"internalType":"address","name":"newOwner","type":"address"}],"name":"OwnerChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DELEGATION_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"DOMAIN_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"abolishSeizing","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_user","type":"address"}],"name":"addToWhitelist","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint32","name":"","type":"uint32"}],"name":"checkpoints","outputs":[{"internalType":"uint32","name":"fromBlock","type":"uint32"},{"internalType":"uint96","name":"votes","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"closeTheGates","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"delegatee","type":"address"}],"name":"delegate","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"delegatee","type":"address"},{"internalType":"uint256","name":"nonce","type":"uint256"},{"internalType":"uint256","name":"expiry","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"delegateBySig","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"delegates","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getCurrentVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"blockNumber","type":"uint256"}],"name":"getPriorVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"mint","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"numCheckpoints","outputs":[{"internalType":"uint32","name":"","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"openTheGates","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_user","type":"address"}],"name":"removeFromWhitelist","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"seizable","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"seize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner_","type":"address"}],"name":"setOwner","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"tradable","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"rawAmount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"whitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H58" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>201</v>
       </c>
@@ -2809,12 +2752,11 @@
       <c r="E59" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="H59" s="0" t="str">
-        <f aca="false">IF(F59="",E59,G59)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"_customTreasury","type":"address"},{"internalType":"address","name":"_payoutToken","type":"address"},{"internalType":"address","name":"_principalToken","type":"address"},{"internalType":"address","name":"_olympusTreasury","type":"address"},{"internalType":"address","name":"_subsidyRouter","type":"address"},{"internalType":"address","name":"_initialOwner","type":"address"},{"internalType":"address","name":"_olympusDAO","type":"address"},{"internalType":"uint256[]","name":"_tierCeilings","type":"uint256[]"},{"internalType":"uint256[]","name":"_fees","type":"uint256[]"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"deposit","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"payout","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"expires","type":"uint256"}],"name":"BondCreated","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"internalPrice","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"debtRatio","type":"uint256"}],"name":"BondPriceChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint256","name":"payout","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"remaining","type":"uint256"}],"name":"BondRedeemed","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"initialBCV","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newBCV","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"adjustment","type":"uint256"},{"indexed":false,"internalType":"bool","name":"addition","type":"bool"}],"name":"ControlVariableAdjustment","type":"event"},{"inputs":[],"name":"adjustment","outputs":[{"internalType":"bool","name":"add","type":"bool"},{"internalType":"uint256","name":"rate","type":"uint256"},{"internalType":"uint256","name":"target","type":"uint256"},{"internalType":"uint256","name":"buffer","type":"uint256"},{"internalType":"uint256","name":"lastBlock","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"bondInfo","outputs":[{"internalType":"uint256","name":"payout","type":"uint256"},{"internalType":"uint256","name":"vesting","type":"uint256"},{"internalType":"uint256","name":"lastBlock","type":"uint256"},{"internalType":"uint256","name":"truePricePaid","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"bondPrice","outputs":[{"internalType":"uint256","name":"price_","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_olympusTreasury","type":"address"}],"name":"changeOlympusTreasury","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"currentDebt","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"currentOlympusFee","outputs":[{"internalType":"uint256","name":"currentFee_","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"debtDecay","outputs":[{"internalType":"uint256","name":"decay_","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"debtRatio","outputs":[{"internalType":"uint256","name":"debtRatio_","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"_amount","type":"uint256"},{"internalType":"uint256","name":"_maxPrice","type":"uint256"},{"internalType":"address","name":"_depositor","type":"address"}],"name":"deposit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_controlVariable","type":"uint256"},{"internalType":"uint256","name":"_vestingTerm","type":"uint256"},{"internalType":"uint256","name":"_minimumPrice","type":"uint256"},{"internalType":"uint256","name":"_maxPayout","type":"uint256"},{"internalType":"uint256","name":"_maxDebt","type":"uint256"},{"internalType":"uint256","name":"_initialDebt","type":"uint256"}],"name":"initializeBond","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"lastDecay","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxPayout","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"paySubsidy","outputs":[{"internalType":"uint256","name":"payoutSinceLastSubsidy_","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_value","type":"uint256"}],"name":"payoutFor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_depositor","type":"address"}],"name":"pendingPayoutFor","outputs":[{"internalType":"uint256","name":"pendingPayout_","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_depositor","type":"address"}],"name":"percentVestedFor","outputs":[{"internalType":"uint256","name":"percentVested_","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"policy","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_depositor","type":"address"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"bool","name":"_addition","type":"bool"},{"internalType":"uint256","name":"_increment","type":"uint256"},{"internalType":"uint256","name":"_target","type":"uint256"},{"internalType":"uint256","name":"_buffer","type":"uint256"}],"name":"setAdjustment","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"enum CustomBond.PARAMETER","name":"_parameter","type":"uint8"},{"internalType":"uint256","name":"_input","type":"uint256"}],"name":"setBondTerms","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"terms","outputs":[{"internalType":"uint256","name":"controlVariable","type":"uint256"},{"internalType":"uint256","name":"vestingTerm","type":"uint256"},{"internalType":"uint256","name":"minimumPrice","type":"uint256"},{"internalType":"uint256","name":"maxPayout","type":"uint256"},{"internalType":"uint256","name":"maxDebt","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalDebt","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalPayoutGiven","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalPrincipalBonded","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_newOwner","type":"address"}],"name":"transferManagment","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"trueBondPrice","outputs":[{"internalType":"uint256","name":"price_","type":"uint256"}],"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H59" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>205</v>
       </c>
@@ -2830,12 +2772,11 @@
       <c r="E60" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="H60" s="0" t="str">
-        <f aca="false">IF(F60="",E60,G60)</f>
-        <v>[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"},{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldImplementation","type":"address"},{"indexed":false,"internalType":"address","name":"newImplementation","type":"address"}],"name":"NewImplementation","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"addAmount","type":"uint256"}],"name":"_addReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"implementation_","type":"address"},{"internalType":"bool","name":"allowResign","type":"bool"},{"internalType":"bytes","name":"becomeImplementationData","type":"bytes"}],"name":"_setImplementation","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"delegateToImplementation","outputs":[{"internalType":"bytes","name":"","type":"bytes"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"bytes","name":"data","type":"bytes"}],"name":"delegateToViewImplementation","outputs":[{"internalType":"bytes","name":"","type":"bytes"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"implementation","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H60" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>209</v>
       </c>
@@ -2851,12 +2792,11 @@
       <c r="E61" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H61" s="0" t="str">
-        <f aca="false">IF(F61="",E61,G61)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H61" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>213</v>
       </c>
@@ -2872,12 +2812,11 @@
       <c r="E62" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H62" s="0" t="str">
-        <f aca="false">IF(F62="",E62,G62)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H62" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>216</v>
       </c>
@@ -2893,12 +2832,11 @@
       <c r="E63" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H63" s="0" t="str">
-        <f aca="false">IF(F63="",E63,G63)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H63" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>219</v>
       </c>
@@ -2914,12 +2852,11 @@
       <c r="E64" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H64" s="0" t="str">
-        <f aca="false">IF(F64="",E64,G64)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H64" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>222</v>
       </c>
@@ -2935,12 +2872,11 @@
       <c r="E65" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H65" s="0" t="str">
-        <f aca="false">IF(F65="",E65,G65)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H65" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>225</v>
       </c>
@@ -2956,12 +2892,11 @@
       <c r="E66" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H66" s="0" t="str">
-        <f aca="false">IF(F66="",E66,G66)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H66" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>228</v>
       </c>
@@ -2977,12 +2912,11 @@
       <c r="E67" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="H67" s="0" t="str">
-        <f aca="false">IF(F67="",E67,G67)</f>
-        <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H67" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>231</v>
       </c>
@@ -2998,12 +2932,11 @@
       <c r="E68" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="H68" s="0" t="str">
-        <f aca="false">IF(F68="",E68,G68)</f>
-        <v>[{"constant":true,"inputs":[],"name":"name","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"spender","type":"address"},{"name":"amount","type":"uint256"}],"name":"approve","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"mint","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"src","type":"address"},{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"repayBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"initialExchangeRateMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"},{"name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"liquidator","type":"address"},{"name":"borrower","type":"address"},{"name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"},{"name":"spender","type":"address"}],"name":"allowance","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"}],"name":"repayBorrowBehalf","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"inputs":[{"name":"comptroller_","type":"address"},{"name":"interestRateModel_","type":"address"},{"name":"initialExchangeRateMantissa_","type":"uint256"},{"name":"name_","type":"string"},{"name":"symbol_","type":"string"},{"name":"decimals_","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"anonymous":false,"inputs":[{"indexed":false,"name":"interestAccumulated","type":"uint256"},{"indexed":false,"name":"borrowIndex","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"minter","type":"address"},{"indexed":false,"name":"mintAmount","type":"uint256"},{"indexed":false,"name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"redeemer","type":"address"},{"indexed":false,"name":"redeemAmount","type":"uint256"},{"indexed":false,"name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"borrowAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"payer","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"liquidator","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"cTokenCollateral","type":"address"},{"indexed":false,"name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldPendingAdmin","type":"address"},{"indexed":false,"name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldAdmin","type":"address"},{"indexed":false,"name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldComptroller","type":"address"},{"indexed":false,"name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldInterestRateModel","type":"address"},{"indexed":false,"name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"admin","type":"address"},{"indexed":false,"name":"reduceAmount","type":"uint256"},{"indexed":false,"name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"error","type":"uint256"},{"indexed":false,"name":"info","type":"uint256"},{"indexed":false,"name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"from","type":"address"},{"indexed":true,"name":"to","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"owner","type":"address"},{"indexed":true,"name":"spender","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Approval","type":"event"}]</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H68" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>235</v>
       </c>
@@ -3019,12 +2952,11 @@
       <c r="E69" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="H69" s="0" t="str">
-        <f aca="false">IF(F69="",E69,G69)</f>
-        <v>[{"constant":true,"inputs":[],"name":"name","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"spender","type":"address"},{"name":"amount","type":"uint256"}],"name":"approve","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"mint","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"src","type":"address"},{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"repayBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"initialExchangeRateMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"},{"name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"liquidator","type":"address"},{"name":"borrower","type":"address"},{"name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"},{"name":"spender","type":"address"}],"name":"allowance","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"}],"name":"repayBorrowBehalf","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"inputs":[{"name":"comptroller_","type":"address"},{"name":"interestRateModel_","type":"address"},{"name":"initialExchangeRateMantissa_","type":"uint256"},{"name":"name_","type":"string"},{"name":"symbol_","type":"string"},{"name":"decimals_","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"anonymous":false,"inputs":[{"indexed":false,"name":"interestAccumulated","type":"uint256"},{"indexed":false,"name":"borrowIndex","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"minter","type":"address"},{"indexed":false,"name":"mintAmount","type":"uint256"},{"indexed":false,"name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"redeemer","type":"address"},{"indexed":false,"name":"redeemAmount","type":"uint256"},{"indexed":false,"name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"borrowAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"payer","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"liquidator","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"cTokenCollateral","type":"address"},{"indexed":false,"name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldPendingAdmin","type":"address"},{"indexed":false,"name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldAdmin","type":"address"},{"indexed":false,"name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldComptroller","type":"address"},{"indexed":false,"name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldInterestRateModel","type":"address"},{"indexed":false,"name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"admin","type":"address"},{"indexed":false,"name":"reduceAmount","type":"uint256"},{"indexed":false,"name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"error","type":"uint256"},{"indexed":false,"name":"info","type":"uint256"},{"indexed":false,"name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"from","type":"address"},{"indexed":true,"name":"to","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"owner","type":"address"},{"indexed":true,"name":"spender","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Approval","type":"event"}]</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H69" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>238</v>
       </c>
@@ -3040,12 +2972,11 @@
       <c r="E70" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="H70" s="0" t="str">
-        <f aca="false">IF(F70="",E70,G70)</f>
-        <v>[{"constant":true,"inputs":[],"name":"name","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"spender","type":"address"},{"name":"amount","type":"uint256"}],"name":"approve","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"mint","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"src","type":"address"},{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"repayBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"initialExchangeRateMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"},{"name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"liquidator","type":"address"},{"name":"borrower","type":"address"},{"name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"},{"name":"spender","type":"address"}],"name":"allowance","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"}],"name":"repayBorrowBehalf","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"inputs":[{"name":"comptroller_","type":"address"},{"name":"interestRateModel_","type":"address"},{"name":"initialExchangeRateMantissa_","type":"uint256"},{"name":"name_","type":"string"},{"name":"symbol_","type":"string"},{"name":"decimals_","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"anonymous":false,"inputs":[{"indexed":false,"name":"interestAccumulated","type":"uint256"},{"indexed":false,"name":"borrowIndex","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"minter","type":"address"},{"indexed":false,"name":"mintAmount","type":"uint256"},{"indexed":false,"name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"redeemer","type":"address"},{"indexed":false,"name":"redeemAmount","type":"uint256"},{"indexed":false,"name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"borrowAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"payer","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"liquidator","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"cTokenCollateral","type":"address"},{"indexed":false,"name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldPendingAdmin","type":"address"},{"indexed":false,"name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldAdmin","type":"address"},{"indexed":false,"name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldComptroller","type":"address"},{"indexed":false,"name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldInterestRateModel","type":"address"},{"indexed":false,"name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"admin","type":"address"},{"indexed":false,"name":"reduceAmount","type":"uint256"},{"indexed":false,"name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"error","type":"uint256"},{"indexed":false,"name":"info","type":"uint256"},{"indexed":false,"name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"from","type":"address"},{"indexed":true,"name":"to","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"owner","type":"address"},{"indexed":true,"name":"spender","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Approval","type":"event"}]</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H70" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>241</v>
       </c>
@@ -3058,9 +2989,8 @@
       <c r="E71" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="H71" s="0" t="str">
-        <f aca="false">IF(F71="",E71,G71)</f>
-        <v>[{"constant":true,"inputs":[],"name":"name","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"spender","type":"address"},{"name":"amount","type":"uint256"}],"name":"approve","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"mint","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"src","type":"address"},{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"repayBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"initialExchangeRateMantissa","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"dst","type":"address"},{"name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"},{"name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"liquidator","type":"address"},{"name":"borrower","type":"address"},{"name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"},{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"owner","type":"address"},{"name":"spender","type":"address"}],"name":"allowance","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"borrower","type":"address"}],"name":"repayBorrowBehalf","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"inputs":[{"name":"comptroller_","type":"address"},{"name":"interestRateModel_","type":"address"},{"name":"initialExchangeRateMantissa_","type":"uint256"},{"name":"name_","type":"string"},{"name":"symbol_","type":"string"},{"name":"decimals_","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"anonymous":false,"inputs":[{"indexed":false,"name":"interestAccumulated","type":"uint256"},{"indexed":false,"name":"borrowIndex","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"minter","type":"address"},{"indexed":false,"name":"mintAmount","type":"uint256"},{"indexed":false,"name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"redeemer","type":"address"},{"indexed":false,"name":"redeemAmount","type":"uint256"},{"indexed":false,"name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"borrowAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"payer","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"accountBorrows","type":"uint256"},{"indexed":false,"name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"liquidator","type":"address"},{"indexed":false,"name":"borrower","type":"address"},{"indexed":false,"name":"repayAmount","type":"uint256"},{"indexed":false,"name":"cTokenCollateral","type":"address"},{"indexed":false,"name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldPendingAdmin","type":"address"},{"indexed":false,"name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldAdmin","type":"address"},{"indexed":false,"name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldComptroller","type":"address"},{"indexed":false,"name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldInterestRateModel","type":"address"},{"indexed":false,"name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"admin","type":"address"},{"indexed":false,"name":"reduceAmount","type":"uint256"},{"indexed":false,"name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"name":"error","type":"uint256"},{"indexed":false,"name":"info","type":"uint256"},{"indexed":false,"name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"from","type":"address"},{"indexed":true,"name":"to","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"owner","type":"address"},{"indexed":true,"name":"spender","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Approval","type":"event"}]</v>
+      <c r="H71" s="0" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Refactor use of view state
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -194,19 +194,19 @@
     <t xml:space="preserve">[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"uint256","name":"rewardPerBlock_","type":"uint256"},{"internalType":"address","name":"rewardTreasury_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegator","type":"address"},{"indexed":true,"internalType":"address","name":"fromDelegate","type":"address"},{"indexed":true,"internalType":"address","name":"toDelegate","type":"address"}],"name":"DelegateChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegate","type":"address"},{"indexed":false,"internalType":"uint256","name":"previousBalance","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newBalance","type":"uint256"}],"name":"DelegateVotesChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldRewardPerBlock","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newRewardPerBlock","type":"uint256"}],"name":"NewRewardPerBlock","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldRewardTreasury","type":"address"},{"indexed":false,"internalType":"address","name":"newRewardTreasury","type":"address"}],"name":"NewRewardTreasury","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract TimelockEscrow","name":"oldTimelockEscrow","type":"address"},{"indexed":false,"internalType":"contract TimelockEscrow","name":"newTimelockEscrow","type":"address"}],"name":"NewTimelockEscrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newRewardPerBlock","type":"uint256"}],"name":"_setRewardPerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newRewardTreasury","type":"address"}],"name":"_setRewardTreasury","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract TimelockEscrow","name":"newTimelockEscrow","type":"address"}],"name":"_setTimelockEscrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint32","name":"","type":"uint32"}],"name":"checkpoints","outputs":[{"internalType":"uint32","name":"fromBlock","type":"uint32"},{"internalType":"uint96","name":"votes","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"delegates","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"escrow","outputs":[{"internalType":"contract TimelockEscrow","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getCurrentVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"blockNumber","type":"uint256"}],"name":"getPriorVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"numCheckpoints","outputs":[{"internalType":"uint32","name":"","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"rewardPerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"rewardTreasury","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"user","type":"address"}],"name":"syncDelegate","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</t>
   </si>
   <si>
+    <t xml:space="preserve">https://etherscan.io/address/0x1637e4e9941d55703a7a5e7807d6ada3f7dcd61b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xe8929afd47064efd36a7fb51da3f8c5eb40c4cb4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anDOLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x7fcb7dac61ee35b3d4a51117a7c58d53f0a8a670</t>
+  </si>
+  <si>
     <t xml:space="preserve">[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"cashPrior","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"interestAccumulated","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"borrowIndex","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"AccrueInterest","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"borrowAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"Borrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"liquidator","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"address","name":"cTokenCollateral","type":"address"},{"indexed":false,"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"LiquidateBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract InterestRateModel","name":"oldInterestRateModel","type":"address"},{"indexed":false,"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"NewMarketInterestRateModel","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldReserveFactorMantissa","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"NewReserveFactor","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"payer","type":"address"},{"indexed":false,"internalType":"address","name":"borrower","type":"address"},{"indexed":false,"internalType":"uint256","name":"repayAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"accountBorrows","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"totalBorrows","type":"uint256"}],"name":"RepayBorrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"benefactor","type":"address"},{"indexed":false,"internalType":"uint256","name":"addAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesAdded","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"admin","type":"address"},{"indexed":false,"internalType":"uint256","name":"reduceAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newTotalReserves","type":"uint256"}],"name":"ReservesReduced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"addAmount","type":"uint256"}],"name":"_addReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"reduceAmount","type":"uint256"}],"name":"_reduceReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract InterestRateModel","name":"newInterestRateModel","type":"address"}],"name":"_setInterestRateModel","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newReserveFactorMantissa","type":"uint256"}],"name":"_setReserveFactor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"borrowAmount","type":"uint256"}],"name":"borrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"borrowBalanceStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"borrowRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"contract InterestRateModel","name":"interestRateModel_","type":"address"},{"internalType":"uint256","name":"initialExchangeRateMantissa_","type":"uint256"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"interestRateModel","outputs":[{"internalType":"contract InterestRateModel","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"},{"internalType":"contract CTokenInterface","name":"cTokenCollateral","type":"address"}],"name":"liquidateBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"repayAmount","type":"uint256"}],"name":"repayBorrowBehalf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"reserveFactorMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"supplyRatePerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalBorrows","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"totalBorrowsCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalReserves","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"src","type":"address"},{"internalType":"address","name":"dst","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://etherscan.io/address/0x1637e4e9941d55703a7a5e7807d6ada3f7dcd61b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xe8929afd47064efd36a7fb51da3f8c5eb40c4cb4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anDOLA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x7fcb7dac61ee35b3d4a51117a7c58d53f0a8a670</t>
   </si>
   <si>
     <t xml:space="preserve">For lending markets use anDOLA ABI</t>
@@ -1750,7 +1750,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="G11 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1809,8 +1809,8 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2099,27 +2099,27 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>21</v>
@@ -2128,13 +2128,13 @@
         <v>59</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>60</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2148,20 +2148,20 @@
         <v>52</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>63</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,20 +2175,20 @@
         <v>52</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>66</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,20 +2202,20 @@
         <v>52</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>69</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,20 +2229,20 @@
         <v>52</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>72</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,20 +2256,20 @@
         <v>52</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>75</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,20 +2283,20 @@
         <v>52</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>78</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2310,20 +2310,20 @@
         <v>52</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>81</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,20 +2337,20 @@
         <v>52</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>84</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,7 +2590,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="G11 F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2744,7 +2744,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2913,8 +2913,8 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="1" sqref="G11 G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2959,7 +2959,7 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q32" activeCellId="0" sqref="Q32"/>
+      <selection pane="topLeft" activeCell="Q32" activeCellId="1" sqref="G11 Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3578,10 +3578,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>251</v>
@@ -3590,10 +3590,10 @@
         <v>52</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,10 +3610,10 @@
         <v>52</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3630,10 +3630,10 @@
         <v>52</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5086,7 +5086,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
+      <selection pane="topLeft" activeCell="I34" activeCellId="1" sqref="G11 I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5110,7 +5110,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Housekeeping, naming multisig alerts
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contracts" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="514">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t xml:space="preserve">0x6c3f90f043a72fa612cbac8115ee7e52bde6e490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt Repayer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9eb6BF2E582279cfC1988d3F2043Ff4DF18fa6A0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"inputs":[{"internalType":"uint256","name":"decimals","type":"uint256"},{"internalType":"uint256","name":"maxDiscount_","type":"uint256"},{"internalType":"uint256","name":"zeroDiscountReserveThreshold_","type":"uint256"},{"internalType":"address","name":"governance_","type":"address"},{"internalType":"address","name":"controller_","type":"address"},{"internalType":"address","name":"treasury_","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"underlying","type":"address"},{"indexed":false,"internalType":"uint256","name":"receiveAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paidAmount","type":"uint256"}],"name":"debtRepayment","type":"event"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"contract IERC20","name":"underlying","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"amountOut","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anBtc","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anEth","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anYfi","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"baseline","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"controller","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"convertToUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"}],"name":"currentDiscount","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"governance","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxDiscount","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"}],"name":"remainingDebt","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"uint256","name":"minOut","type":"uint256"}],"name":"sellDebt","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newController","type":"address"}],"name":"setController","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newGovernance","type":"address"}],"name":"setGovernance","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"newMaxDiscount","type":"uint256"}],"name":"setMaxDiscount","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newTreasury","type":"address"}],"name":"setTreasury","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"newZeroDiscountReserveThreshold","type":"uint256"}],"name":"setZeroDiscountReserveThreshold","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"token","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"sweepTokens","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"treasury","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"zeroDiscountReserveThreshold","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"stateMutability":"payable","type":"receive"}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repayment</t>
   </si>
   <si>
     <t xml:space="preserve">lending2</t>
@@ -1807,10 +1819,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1845,6 +1853,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1973,8 +1985,8 @@
   </sheetPr>
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2750,62 +2762,82 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="4" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="E39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="E40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="E41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2840,8 +2872,8 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2850,151 +2882,152 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>119</v>
       </c>
+      <c r="E2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="11"/>
+      <c r="D3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="11"/>
+      <c r="A4" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="A5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="A6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3025,61 +3058,61 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>137</v>
+      <c r="A2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3111,47 +3144,47 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3189,19 +3222,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -3209,16 +3242,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>61</v>
@@ -3236,10 +3269,10 @@
         <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>146</v>
+        <v>151</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>77</v>
@@ -3251,19 +3284,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>146</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">IF(F4="",E4,G4)</f>
@@ -3272,19 +3305,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>146</v>
+        <v>158</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H5" s="0" t="str">
         <f aca="false">IF(F5="",E5,G5)</f>
@@ -3293,19 +3326,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>151</v>
       </c>
       <c r="H6" s="0" t="str">
         <f aca="false">IF(F6="",E6,G6)</f>
@@ -3314,19 +3347,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>146</v>
+        <v>164</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H7" s="0" t="str">
         <f aca="false">IF(F7="",E7,G7)</f>
@@ -3335,19 +3368,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>146</v>
+        <v>167</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H8" s="0" t="str">
         <f aca="false">IF(F8="",E8,G8)</f>
@@ -3356,19 +3389,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>146</v>
+        <v>170</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H9" s="0" t="str">
         <f aca="false">IF(F9="",E9,G9)</f>
@@ -3377,19 +3410,19 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>146</v>
+        <v>173</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H10" s="0" t="str">
         <f aca="false">IF(F10="",E10,G10)</f>
@@ -3398,19 +3431,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>146</v>
+        <v>176</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H11" s="0" t="str">
         <f aca="false">IF(F11="",E11,G11)</f>
@@ -3419,19 +3452,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>146</v>
+        <v>179</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">IF(F12="",E12,G12)</f>
@@ -3440,19 +3473,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>146</v>
+        <v>182</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H13" s="0" t="str">
         <f aca="false">IF(F13="",E13,G13)</f>
@@ -3461,19 +3494,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>146</v>
+        <v>185</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H14" s="0" t="str">
         <f aca="false">IF(F14="",E14,G14)</f>
@@ -3482,19 +3515,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>146</v>
+        <v>188</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">IF(F15="",E15,G15)</f>
@@ -3503,19 +3536,19 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>146</v>
+        <v>191</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">IF(F16="",E16,G16)</f>
@@ -3524,19 +3557,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>146</v>
+        <v>195</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">IF(F17="",E17,G17)</f>
@@ -3545,19 +3578,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>192</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>188</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">IF(F18="",E18,G18)</f>
@@ -3572,10 +3605,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>146</v>
+        <v>199</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>36</v>
@@ -3587,19 +3620,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>146</v>
+        <v>201</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">IF(F20="",E20,G20)</f>
@@ -3608,19 +3641,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="H21" s="0" t="str">
         <f aca="false">IF(F21="",E21,G21)</f>
@@ -3629,19 +3662,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>207</v>
+      <c r="E22" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">IF(F22="",E22,G22)</f>
@@ -3650,19 +3683,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>211</v>
+        <v>214</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="H23" s="0" t="str">
         <f aca="false">IF(F23="",E23,G23)</f>
@@ -3671,19 +3704,19 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>219</v>
       </c>
       <c r="H24" s="0" t="str">
         <f aca="false">IF(F24="",E24,G24)</f>
@@ -3692,22 +3725,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>202</v>
+        <v>222</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3718,10 +3751,10 @@
         <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>202</v>
+        <v>224</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>106</v>
@@ -3738,10 +3771,10 @@
         <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>146</v>
+        <v>225</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>77</v>
@@ -3758,10 +3791,10 @@
         <v>17</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>146</v>
+        <v>226</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>18</v>
@@ -3778,16 +3811,16 @@
         <v>68</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>146</v>
+        <v>227</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,10 +3831,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>226</v>
+        <v>229</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>41</v>
@@ -3818,10 +3851,10 @@
         <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>226</v>
+        <v>231</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>41</v>
@@ -3838,10 +3871,10 @@
         <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>226</v>
+        <v>232</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>41</v>
@@ -3858,16 +3891,16 @@
         <v>48</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>226</v>
+        <v>233</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3878,10 +3911,10 @@
         <v>50</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>226</v>
+        <v>235</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>101</v>
@@ -3892,16 +3925,16 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>146</v>
+        <v>238</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>106</v>
@@ -3912,22 +3945,22 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>146</v>
+        <v>241</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3938,10 +3971,10 @@
         <v>12</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>111</v>
+        <v>242</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>13</v>
@@ -3952,594 +3985,594 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>146</v>
+        <v>245</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>226</v>
+        <v>249</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="F40" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>247</v>
-      </c>
       <c r="G40" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="G41" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>248</v>
-      </c>
       <c r="H41" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>226</v>
+        <v>262</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>226</v>
+        <v>265</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>226</v>
+        <v>268</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>226</v>
+        <v>271</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>226</v>
+        <v>274</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>226</v>
+        <v>277</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>226</v>
+        <v>280</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>226</v>
+        <v>283</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>226</v>
+        <v>287</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>226</v>
+        <v>291</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>226</v>
+        <v>294</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>226</v>
+        <v>297</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>226</v>
+        <v>300</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>226</v>
+        <v>303</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>226</v>
+        <v>306</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>226</v>
+        <v>309</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>226</v>
+        <v>312</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>226</v>
+        <v>315</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>226</v>
+        <v>318</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4550,10 +4583,10 @@
         <v>21</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>146</v>
+        <v>319</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>22</v>
@@ -4570,10 +4603,10 @@
         <v>21</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>146</v>
+        <v>319</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>22</v>
@@ -4584,172 +4617,172 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>226</v>
+        <v>322</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>226</v>
+        <v>325</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>226</v>
+        <v>328</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>226</v>
+        <v>331</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>146</v>
+        <v>333</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>146</v>
+        <v>336</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>69</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C69" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="F69" s="0" t="s">
         <v>335</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>331</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>69</v>
@@ -4760,22 +4793,22 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>146</v>
+        <v>343</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>69</v>
@@ -4786,22 +4819,22 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>146</v>
+        <v>347</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>69</v>
@@ -4812,22 +4845,22 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="B72" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="D72" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>340</v>
-      </c>
       <c r="F72" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>69</v>
@@ -4844,10 +4877,10 @@
         <v>27</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>146</v>
+        <v>351</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>18</v>
@@ -4864,10 +4897,10 @@
         <v>29</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>146</v>
+        <v>352</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>18</v>
@@ -4884,10 +4917,10 @@
         <v>31</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>146</v>
+        <v>353</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>18</v>
@@ -4904,10 +4937,10 @@
         <v>33</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>146</v>
+        <v>354</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>18</v>
@@ -4918,154 +4951,154 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>226</v>
+        <v>357</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>226</v>
+        <v>360</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>226</v>
+        <v>360</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>146</v>
+        <v>364</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>146</v>
+        <v>367</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>146</v>
+        <v>371</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>146</v>
+        <v>375</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>61</v>
@@ -5082,10 +5115,10 @@
         <v>60</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>372</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>146</v>
+        <v>376</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>61</v>
@@ -5102,10 +5135,10 @@
         <v>64</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>146</v>
+        <v>377</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>61</v>
@@ -5116,16 +5149,16 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>146</v>
+        <v>380</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>61</v>
@@ -5136,16 +5169,16 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>146</v>
+        <v>383</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>61</v>
@@ -5156,16 +5189,16 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>146</v>
+        <v>386</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>61</v>
@@ -5176,16 +5209,16 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D89" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>61</v>
@@ -5196,82 +5229,82 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="D90" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>386</v>
+        <v>389</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>386</v>
+        <v>393</v>
+      </c>
+      <c r="D91" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E92" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>386</v>
-      </c>
       <c r="H92" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="D93" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>386</v>
+        <v>399</v>
+      </c>
+      <c r="D93" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5279,18 +5312,18 @@
         <v>102</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>399</v>
+        <v>402</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>403</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>77</v>
@@ -5302,15 +5335,15 @@
         <v>10</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>402</v>
+        <v>405</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>406</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>77</v>
@@ -5322,15 +5355,15 @@
         <v>10</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>404</v>
+        <v>407</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>408</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>77</v>
@@ -5342,15 +5375,15 @@
         <v>10</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>406</v>
+        <v>409</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>410</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>77</v>
@@ -5362,15 +5395,15 @@
         <v>10</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>408</v>
+        <v>411</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>412</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>77</v>
@@ -5382,15 +5415,15 @@
         <v>10</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>410</v>
+        <v>413</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>414</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>77</v>
@@ -5402,15 +5435,15 @@
         <v>10</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>412</v>
+        <v>415</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>416</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>77</v>
@@ -5422,15 +5455,15 @@
         <v>10</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>414</v>
+        <v>417</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>418</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>77</v>
@@ -5442,15 +5475,15 @@
         <v>10</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>416</v>
+        <v>419</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>420</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>77</v>
@@ -5462,15 +5495,15 @@
         <v>10</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>418</v>
+        <v>421</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>422</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>77</v>
@@ -5482,15 +5515,15 @@
         <v>10</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>420</v>
+        <v>423</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>424</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>77</v>
@@ -5502,15 +5535,15 @@
         <v>10</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>422</v>
+        <v>425</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>426</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>77</v>
@@ -5522,15 +5555,15 @@
         <v>10</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>423</v>
-      </c>
-      <c r="B107" s="9" t="s">
-        <v>424</v>
+        <v>427</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>428</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>77</v>
@@ -5542,15 +5575,15 @@
         <v>10</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>426</v>
+        <v>429</v>
+      </c>
+      <c r="B108" s="18" t="s">
+        <v>430</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>77</v>
@@ -5562,15 +5595,15 @@
         <v>10</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="B109" s="9" t="s">
-        <v>428</v>
+        <v>431</v>
+      </c>
+      <c r="B109" s="18" t="s">
+        <v>432</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>77</v>
@@ -5582,15 +5615,15 @@
         <v>10</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>429</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>430</v>
+        <v>433</v>
+      </c>
+      <c r="B110" s="18" t="s">
+        <v>434</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>77</v>
@@ -5602,15 +5635,15 @@
         <v>10</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>432</v>
+        <v>435</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>436</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>77</v>
@@ -5622,15 +5655,15 @@
         <v>10</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>434</v>
+        <v>437</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>438</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>77</v>
@@ -5642,15 +5675,15 @@
         <v>10</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>436</v>
+        <v>439</v>
+      </c>
+      <c r="B113" s="18" t="s">
+        <v>440</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>77</v>
@@ -5662,15 +5695,15 @@
         <v>10</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>438</v>
+        <v>441</v>
+      </c>
+      <c r="B114" s="18" t="s">
+        <v>442</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>77</v>
@@ -5682,15 +5715,15 @@
         <v>10</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>440</v>
+        <v>443</v>
+      </c>
+      <c r="B115" s="18" t="s">
+        <v>444</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>77</v>
@@ -5702,15 +5735,15 @@
         <v>10</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="B116" s="9" t="s">
-        <v>442</v>
+        <v>445</v>
+      </c>
+      <c r="B116" s="18" t="s">
+        <v>446</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>77</v>
@@ -5722,15 +5755,15 @@
         <v>10</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>443</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>444</v>
+        <v>447</v>
+      </c>
+      <c r="B117" s="18" t="s">
+        <v>448</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>77</v>
@@ -5742,15 +5775,15 @@
         <v>10</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>446</v>
+        <v>449</v>
+      </c>
+      <c r="B118" s="18" t="s">
+        <v>450</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>77</v>
@@ -5762,15 +5795,15 @@
         <v>10</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>447</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>448</v>
+        <v>451</v>
+      </c>
+      <c r="B119" s="18" t="s">
+        <v>452</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>77</v>
@@ -5782,15 +5815,15 @@
         <v>10</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>450</v>
+        <v>453</v>
+      </c>
+      <c r="B120" s="18" t="s">
+        <v>454</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>77</v>
@@ -5802,15 +5835,15 @@
         <v>10</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>451</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>452</v>
+        <v>455</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>456</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>77</v>
@@ -5822,15 +5855,15 @@
         <v>10</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>454</v>
+        <v>457</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>458</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>77</v>
@@ -5842,15 +5875,15 @@
         <v>10</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
+      </c>
+      <c r="B123" s="18" t="s">
+        <v>460</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>77</v>
@@ -5862,15 +5895,15 @@
         <v>10</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>458</v>
+        <v>461</v>
+      </c>
+      <c r="B124" s="18" t="s">
+        <v>462</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>77</v>
@@ -5882,15 +5915,15 @@
         <v>10</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>460</v>
+        <v>463</v>
+      </c>
+      <c r="B125" s="18" t="s">
+        <v>464</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>77</v>
@@ -5902,15 +5935,15 @@
         <v>10</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>461</v>
-      </c>
-      <c r="B126" s="9" t="s">
-        <v>462</v>
+        <v>465</v>
+      </c>
+      <c r="B126" s="18" t="s">
+        <v>466</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>77</v>
@@ -5922,15 +5955,15 @@
         <v>10</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>463</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>464</v>
+        <v>467</v>
+      </c>
+      <c r="B127" s="18" t="s">
+        <v>468</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>77</v>
@@ -5942,15 +5975,15 @@
         <v>10</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>465</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>466</v>
+        <v>469</v>
+      </c>
+      <c r="B128" s="18" t="s">
+        <v>470</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>77</v>
@@ -5962,15 +5995,15 @@
         <v>10</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="B129" s="9" t="s">
-        <v>468</v>
+        <v>471</v>
+      </c>
+      <c r="B129" s="18" t="s">
+        <v>472</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>77</v>
@@ -5982,15 +6015,15 @@
         <v>10</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>470</v>
+        <v>473</v>
+      </c>
+      <c r="B130" s="18" t="s">
+        <v>474</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>77</v>
@@ -6002,15 +6035,15 @@
         <v>10</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>472</v>
+        <v>475</v>
+      </c>
+      <c r="B131" s="18" t="s">
+        <v>476</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>77</v>
@@ -6022,15 +6055,15 @@
         <v>10</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="B132" s="9" t="s">
-        <v>474</v>
+        <v>477</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>478</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>77</v>
@@ -6042,15 +6075,15 @@
         <v>10</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>476</v>
+        <v>479</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>480</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>77</v>
@@ -6062,15 +6095,15 @@
         <v>10</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>477</v>
-      </c>
-      <c r="B134" s="9" t="s">
-        <v>478</v>
+        <v>481</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>482</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>77</v>
@@ -6082,15 +6115,15 @@
         <v>10</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="B135" s="9" t="s">
-        <v>480</v>
+        <v>483</v>
+      </c>
+      <c r="B135" s="18" t="s">
+        <v>484</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>77</v>
@@ -6102,15 +6135,15 @@
         <v>10</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="B136" s="9" t="s">
-        <v>482</v>
+        <v>485</v>
+      </c>
+      <c r="B136" s="18" t="s">
+        <v>486</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>77</v>
@@ -6122,15 +6155,15 @@
         <v>10</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="B137" s="9" t="s">
-        <v>484</v>
+        <v>487</v>
+      </c>
+      <c r="B137" s="18" t="s">
+        <v>488</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>77</v>
@@ -6142,15 +6175,15 @@
         <v>10</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="B138" s="9" t="s">
-        <v>486</v>
+        <v>489</v>
+      </c>
+      <c r="B138" s="18" t="s">
+        <v>490</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>77</v>
@@ -6162,15 +6195,15 @@
         <v>10</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="B139" s="9" t="s">
-        <v>488</v>
+        <v>491</v>
+      </c>
+      <c r="B139" s="18" t="s">
+        <v>492</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>77</v>
@@ -6182,15 +6215,15 @@
         <v>10</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>489</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>490</v>
+        <v>493</v>
+      </c>
+      <c r="B140" s="18" t="s">
+        <v>494</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>77</v>
@@ -6202,15 +6235,15 @@
         <v>10</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="B141" s="9" t="s">
-        <v>492</v>
+        <v>495</v>
+      </c>
+      <c r="B141" s="18" t="s">
+        <v>496</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>77</v>
@@ -6222,15 +6255,15 @@
         <v>10</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>493</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>494</v>
+        <v>497</v>
+      </c>
+      <c r="B142" s="18" t="s">
+        <v>498</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>77</v>
@@ -6242,15 +6275,15 @@
         <v>10</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>495</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>496</v>
+        <v>499</v>
+      </c>
+      <c r="B143" s="18" t="s">
+        <v>500</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>77</v>
@@ -6262,15 +6295,15 @@
         <v>10</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>497</v>
-      </c>
-      <c r="B144" s="9" t="s">
-        <v>498</v>
+        <v>501</v>
+      </c>
+      <c r="B144" s="18" t="s">
+        <v>502</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>77</v>
@@ -6282,15 +6315,15 @@
         <v>10</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>500</v>
+        <v>503</v>
+      </c>
+      <c r="B145" s="18" t="s">
+        <v>504</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>77</v>
@@ -6302,15 +6335,15 @@
         <v>10</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="B146" s="9" t="s">
-        <v>502</v>
+        <v>505</v>
+      </c>
+      <c r="B146" s="18" t="s">
+        <v>506</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>77</v>
@@ -6322,15 +6355,15 @@
         <v>10</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>504</v>
+        <v>507</v>
+      </c>
+      <c r="B147" s="18" t="s">
+        <v>508</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>77</v>
@@ -6342,15 +6375,15 @@
         <v>10</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>505</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>506</v>
+        <v>509</v>
+      </c>
+      <c r="B148" s="18" t="s">
+        <v>510</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>77</v>
@@ -6362,21 +6395,21 @@
         <v>10</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Add debt conversion events
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="520">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -368,7 +368,19 @@
     <t xml:space="preserve">[{"inputs":[{"internalType":"uint256","name":"decimals","type":"uint256"},{"internalType":"uint256","name":"maxDiscount_","type":"uint256"},{"internalType":"uint256","name":"zeroDiscountReserveThreshold_","type":"uint256"},{"internalType":"address","name":"governance_","type":"address"},{"internalType":"address","name":"controller_","type":"address"},{"internalType":"address","name":"treasury_","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"underlying","type":"address"},{"indexed":false,"internalType":"uint256","name":"receiveAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paidAmount","type":"uint256"}],"name":"debtRepayment","type":"event"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"contract IERC20","name":"underlying","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"amountOut","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anBtc","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anEth","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anYfi","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"baseline","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"controller","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"convertToUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"}],"name":"currentDiscount","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"governance","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxDiscount","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"}],"name":"remainingDebt","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"uint256","name":"minOut","type":"uint256"}],"name":"sellDebt","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newController","type":"address"}],"name":"setController","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newGovernance","type":"address"}],"name":"setGovernance","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"newMaxDiscount","type":"uint256"}],"name":"setMaxDiscount","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newTreasury","type":"address"}],"name":"setTreasury","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"newZeroDiscountReserveThreshold","type":"uint256"}],"name":"setZeroDiscountReserveThreshold","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"token","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"sweepTokens","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"treasury","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"zeroDiscountReserveThreshold","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"stateMutability":"payable","type":"receive"}]</t>
   </si>
   <si>
-    <t xml:space="preserve">repayment</t>
+    <t xml:space="preserve">debt_repayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debt Converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1ff9c712B011cBf05B67A6850281b13cA27eCb2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"inputs":[{"internalType":"uint256","name":"initialIncreasePerYear","type":"uint256"},{"internalType":"address","name":"_owner","type":"address"},{"internalType":"address","name":"_treasury","type":"address"},{"internalType":"address","name":"_governance","type":"address"},{"internalType":"address","name":"_oracle","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"inputs":[],"name":"ConversionDoesNotExist","type":"error"},{"inputs":[{"internalType":"uint256","name":"conversionEpoch","type":"uint256"},{"internalType":"uint256","name":"currentEpoch","type":"uint256"}],"name":"ConversionEpochNotEqualToCurrentEpoch","type":"error"},{"inputs":[],"name":"ConversionHasNotBeenRedeemedBefore","type":"error"},{"inputs":[{"internalType":"uint256","name":"minOut","type":"uint256"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"DolaAmountLessThanMinOut","type":"error"},{"inputs":[{"internalType":"uint256","name":"repayment","type":"uint256"},{"internalType":"uint256","name":"debt","type":"uint256"}],"name":"InsufficientDebtToBeRepaid","type":"error"},{"inputs":[{"internalType":"uint256","name":"needed","type":"uint256"},{"internalType":"uint256","name":"actual","type":"uint256"}],"name":"InsufficientDebtTokens","type":"error"},{"inputs":[{"internalType":"uint256","name":"needed","type":"uint256"},{"internalType":"uint256","name":"actual","type":"uint256"}],"name":"InsufficientTreasuryFunds","type":"error"},{"inputs":[],"name":"InvalidDebtToken","type":"error"},{"inputs":[],"name":"OnlyGovernance","type":"error"},{"inputs":[],"name":"OnlyOwner","type":"error"},{"inputs":[],"name":"ThatEpochIsInTheFuture","type":"error"},{"inputs":[],"name":"TransferToAddressNotWhitelisted","type":"error"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"user","type":"address"},{"indexed":true,"internalType":"address","name":"anToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"epoch","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"dolaAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"underlyingAmount","type":"uint256"}],"name":"Conversion","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"increase","type":"uint256"}],"name":"NewAnnualExchangeRateIncrease","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"governance","type":"address"}],"name":"NewGovernance","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"anToken","type":"address"},{"indexed":false,"internalType":"uint256","name":"maxPrice","type":"uint256"}],"name":"NewMaxConvertPrice","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"owner","type":"address"}],"name":"NewOwner","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"whitelistedAddr","type":"address"}],"name":"NewTransferWhitelistAddress","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"treasury","type":"address"}],"name":"NewTreasury","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"user","type":"address"},{"indexed":false,"internalType":"uint256","name":"dolaAmount","type":"uint256"}],"name":"Redemption","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"dolaAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"epoch","type":"uint256"}],"name":"Repayment","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOLA","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"accrueInterest","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anBtc","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anEth","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"anYfi","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_addr","type":"address"}],"name":"balanceOfDola","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint256","name":"","type":"uint256"}],"name":"conversions","outputs":[{"internalType":"uint256","name":"lastEpochRedeemed","type":"uint256"},{"internalType":"uint256","name":"dolaIOUAmount","type":"uint256"},{"internalType":"uint256","name":"dolaIOUsRedeemed","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"},{"internalType":"uint256","name":"minOut","type":"uint256"}],"name":"convert","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"dolaIOUs","type":"uint256"}],"name":"convertDolaIOUsToDola","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"dola","type":"uint256"}],"name":"convertDolaToDolaIOUs","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"cumDebt","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"cumDolaRepaid","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"exchangeRateIncreasePerSecond","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"exchangeRateMantissa","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_addr","type":"address"},{"internalType":"uint256","name":"_conversion","type":"uint256"},{"internalType":"uint256","name":"_epoch","type":"uint256"}],"name":"getRedeemableDolaIOUsFor","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"governance","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"lastAccrueInterestTimestamp","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"maxConvertPrice","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"oracle","outputs":[{"internalType":"contract Ioracle","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"outstandingDebt","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"owner","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"_conversion","type":"uint256"}],"name":"redeemAll","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_conversion","type":"uint256"},{"internalType":"uint256","name":"_endEpoch","type":"uint256"}],"name":"redeemConversion","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_conversion","type":"uint256"}],"name":"redeemConversionDust","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"repayment","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"repaymentEpoch","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"repayments","outputs":[{"internalType":"uint256","name":"epoch","type":"uint256"},{"internalType":"uint256","name":"dolaAmount","type":"uint256"},{"internalType":"uint256","name":"pctDolaIOUsRedeemable","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint256","name":"increasePerYear","type":"uint256"}],"name":"setExchangeRateIncrease","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newGovernance","type":"address"}],"name":"setGovernance","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"anToken","type":"address"},{"internalType":"uint256","name":"maxPrice","type":"uint256"}],"name":"setMaxConvertPrice","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newOwner","type":"address"}],"name":"setOwner","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newTreasury","type":"address"}],"name":"setTreasury","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"token","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"sweepTokens","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"transferWhitelist","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"treasury","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"whitelistedAddress","type":"address"}],"name":"whitelistTransferFor","outputs":[],"stateMutability":"nonpayable","type":"function"}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debt_conversion</t>
   </si>
   <si>
     <t xml:space="preserve">lending2</t>
@@ -399,6 +411,12 @@
   </si>
   <si>
     <t xml:space="preserve">Transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debtRepayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversion</t>
   </si>
   <si>
     <t xml:space="preserve">NewBorrowCap</t>
@@ -1985,8 +2003,8 @@
   </sheetPr>
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1994,7 +2012,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.98"/>
@@ -2838,6 +2856,26 @@
         <v>10</v>
       </c>
       <c r="F42" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2870,10 +2908,10 @@
     <tabColor rgb="FFDDE8CB"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2896,10 +2934,10 @@
         <v>37</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>19</v>
@@ -2910,83 +2948,99 @@
       <c r="H1" s="9" t="s">
         <v>107</v>
       </c>
+      <c r="I1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -2994,10 +3048,12 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -3006,10 +3062,12 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -3018,6 +3076,8 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
@@ -3028,6 +3088,8 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3070,13 +3132,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,10 +3265,10 @@
     <tabColor rgb="FFFFE994"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A125" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A149" activeCellId="0" sqref="A149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H157" activeCellId="0" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3222,19 +3284,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -3242,16 +3304,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>61</v>
@@ -3269,10 +3331,10 @@
         <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>77</v>
@@ -3284,19 +3346,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">IF(F4="",E4,G4)</f>
@@ -3305,19 +3367,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>150</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H5" s="0" t="str">
         <f aca="false">IF(F5="",E5,G5)</f>
@@ -3326,19 +3388,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="H6" s="0" t="str">
         <f aca="false">IF(F6="",E6,G6)</f>
@@ -3347,19 +3409,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H7" s="0" t="str">
         <f aca="false">IF(F7="",E7,G7)</f>
@@ -3368,19 +3430,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H8" s="0" t="str">
         <f aca="false">IF(F8="",E8,G8)</f>
@@ -3389,19 +3451,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H9" s="0" t="str">
         <f aca="false">IF(F9="",E9,G9)</f>
@@ -3410,19 +3472,19 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H10" s="0" t="str">
         <f aca="false">IF(F10="",E10,G10)</f>
@@ -3431,19 +3493,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H11" s="0" t="str">
         <f aca="false">IF(F11="",E11,G11)</f>
@@ -3452,19 +3514,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">IF(F12="",E12,G12)</f>
@@ -3473,19 +3535,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H13" s="0" t="str">
         <f aca="false">IF(F13="",E13,G13)</f>
@@ -3494,19 +3556,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H14" s="0" t="str">
         <f aca="false">IF(F14="",E14,G14)</f>
@@ -3515,19 +3577,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">IF(F15="",E15,G15)</f>
@@ -3536,19 +3598,19 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">IF(F16="",E16,G16)</f>
@@ -3557,19 +3619,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">IF(F17="",E17,G17)</f>
@@ -3578,19 +3640,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>192</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">IF(F18="",E18,G18)</f>
@@ -3605,10 +3667,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>36</v>
@@ -3620,19 +3682,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">IF(F20="",E20,G20)</f>
@@ -3641,19 +3703,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H21" s="0" t="str">
         <f aca="false">IF(F21="",E21,G21)</f>
@@ -3662,19 +3724,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">IF(F22="",E22,G22)</f>
@@ -3683,19 +3745,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>206</v>
-      </c>
       <c r="E23" s="12" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="H23" s="0" t="str">
         <f aca="false">IF(F23="",E23,G23)</f>
@@ -3704,19 +3766,19 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="H24" s="0" t="str">
         <f aca="false">IF(F24="",E24,G24)</f>
@@ -3725,22 +3787,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,10 +3813,10 @@
         <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>106</v>
@@ -3771,10 +3833,10 @@
         <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>77</v>
@@ -3791,10 +3853,10 @@
         <v>17</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>18</v>
@@ -3811,16 +3873,16 @@
         <v>68</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,10 +3893,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>41</v>
@@ -3851,10 +3913,10 @@
         <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>41</v>
@@ -3871,10 +3933,10 @@
         <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>41</v>
@@ -3891,16 +3953,16 @@
         <v>48</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3911,10 +3973,10 @@
         <v>50</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>101</v>
@@ -3925,16 +3987,16 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>106</v>
@@ -3945,22 +4007,22 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,10 +4033,10 @@
         <v>12</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>13</v>
@@ -3985,594 +4047,594 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="G41" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D41" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>252</v>
-      </c>
       <c r="H41" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4583,10 +4645,10 @@
         <v>21</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>22</v>
@@ -4603,10 +4665,10 @@
         <v>21</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>22</v>
@@ -4617,172 +4679,172 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>69</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>69</v>
@@ -4793,22 +4855,22 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="F70" s="0" t="s">
         <v>341</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>335</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>69</v>
@@ -4819,22 +4881,22 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>69</v>
@@ -4845,22 +4907,22 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="C72" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E72" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="D72" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>344</v>
-      </c>
       <c r="F72" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>69</v>
@@ -4877,10 +4939,10 @@
         <v>27</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>18</v>
@@ -4897,10 +4959,10 @@
         <v>29</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>18</v>
@@ -4917,10 +4979,10 @@
         <v>31</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>18</v>
@@ -4937,10 +4999,10 @@
         <v>33</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>18</v>
@@ -4951,154 +5013,154 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="D78" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="D79" s="16" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>61</v>
@@ -5115,10 +5177,10 @@
         <v>60</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>61</v>
@@ -5135,10 +5197,10 @@
         <v>64</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>61</v>
@@ -5149,16 +5211,16 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>61</v>
@@ -5169,16 +5231,16 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>61</v>
@@ -5189,16 +5251,16 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>61</v>
@@ -5209,16 +5271,16 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>61</v>
@@ -5229,82 +5291,82 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="C92" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E92" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="D92" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>390</v>
-      </c>
       <c r="H92" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5312,18 +5374,18 @@
         <v>102</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>77</v>
@@ -5335,15 +5397,15 @@
         <v>10</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>77</v>
@@ -5355,15 +5417,15 @@
         <v>10</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>77</v>
@@ -5375,15 +5437,15 @@
         <v>10</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>77</v>
@@ -5395,15 +5457,15 @@
         <v>10</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>77</v>
@@ -5415,15 +5477,15 @@
         <v>10</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>77</v>
@@ -5435,15 +5497,15 @@
         <v>10</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>77</v>
@@ -5455,15 +5517,15 @@
         <v>10</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>77</v>
@@ -5475,15 +5537,15 @@
         <v>10</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>77</v>
@@ -5495,15 +5557,15 @@
         <v>10</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>77</v>
@@ -5515,15 +5577,15 @@
         <v>10</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>77</v>
@@ -5535,15 +5597,15 @@
         <v>10</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>77</v>
@@ -5555,15 +5617,15 @@
         <v>10</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>77</v>
@@ -5575,15 +5637,15 @@
         <v>10</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>77</v>
@@ -5595,15 +5657,15 @@
         <v>10</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>77</v>
@@ -5615,15 +5677,15 @@
         <v>10</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>77</v>
@@ -5635,15 +5697,15 @@
         <v>10</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>77</v>
@@ -5655,15 +5717,15 @@
         <v>10</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>77</v>
@@ -5675,15 +5737,15 @@
         <v>10</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>77</v>
@@ -5695,15 +5757,15 @@
         <v>10</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>77</v>
@@ -5715,15 +5777,15 @@
         <v>10</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>77</v>
@@ -5735,15 +5797,15 @@
         <v>10</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>77</v>
@@ -5755,15 +5817,15 @@
         <v>10</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>77</v>
@@ -5775,15 +5837,15 @@
         <v>10</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>77</v>
@@ -5795,15 +5857,15 @@
         <v>10</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>77</v>
@@ -5815,15 +5877,15 @@
         <v>10</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>77</v>
@@ -5835,15 +5897,15 @@
         <v>10</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="B121" s="18" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>77</v>
@@ -5855,15 +5917,15 @@
         <v>10</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>77</v>
@@ -5875,15 +5937,15 @@
         <v>10</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>77</v>
@@ -5895,15 +5957,15 @@
         <v>10</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>77</v>
@@ -5915,15 +5977,15 @@
         <v>10</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>77</v>
@@ -5935,15 +5997,15 @@
         <v>10</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>77</v>
@@ -5955,15 +6017,15 @@
         <v>10</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>77</v>
@@ -5975,15 +6037,15 @@
         <v>10</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>77</v>
@@ -5995,15 +6057,15 @@
         <v>10</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="B129" s="18" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>77</v>
@@ -6015,15 +6077,15 @@
         <v>10</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="B130" s="18" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>77</v>
@@ -6035,15 +6097,15 @@
         <v>10</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="B131" s="18" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>77</v>
@@ -6055,15 +6117,15 @@
         <v>10</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B132" s="18" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>77</v>
@@ -6075,15 +6137,15 @@
         <v>10</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="B133" s="18" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>77</v>
@@ -6095,15 +6157,15 @@
         <v>10</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="B134" s="18" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>77</v>
@@ -6115,15 +6177,15 @@
         <v>10</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="B135" s="18" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>77</v>
@@ -6135,15 +6197,15 @@
         <v>10</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B136" s="18" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>77</v>
@@ -6155,15 +6217,15 @@
         <v>10</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>77</v>
@@ -6175,15 +6237,15 @@
         <v>10</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>77</v>
@@ -6195,15 +6257,15 @@
         <v>10</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B139" s="18" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>77</v>
@@ -6215,15 +6277,15 @@
         <v>10</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>77</v>
@@ -6235,15 +6297,15 @@
         <v>10</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B141" s="18" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>77</v>
@@ -6255,15 +6317,15 @@
         <v>10</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>77</v>
@@ -6275,15 +6337,15 @@
         <v>10</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="B143" s="18" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>77</v>
@@ -6295,15 +6357,15 @@
         <v>10</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>77</v>
@@ -6315,15 +6377,15 @@
         <v>10</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>77</v>
@@ -6335,15 +6397,15 @@
         <v>10</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>77</v>
@@ -6355,15 +6417,15 @@
         <v>10</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="B147" s="18" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>77</v>
@@ -6375,15 +6437,15 @@
         <v>10</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>77</v>
@@ -6395,21 +6457,21 @@
         <v>10</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>10</v>
@@ -6418,6 +6480,7 @@
         <v>10</v>
       </c>
     </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C90" r:id="rId1" display="https://etherscan.io/address/0x4ddc2d193948926d02f9b1fe9e1daa0718270ed5"/>

</xml_diff>

<commit_message>
add curve gauge contracts and dolafrax pool
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="contracts" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">contracts!$A$1:$G$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">contracts_deprecated!$A$1:$H$149</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="533">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -402,6 +403,39 @@
   </si>
   <si>
     <t xml:space="preserve">0x814b02c1ebc9164972d888495927fe1697f0fb4c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOLAFRAXBP Pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xE57180685E3348589E9521aa53Af0BCD497E884d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"name":"Transfer","inputs":[{"name":"sender","type":"address","indexed":true},{"name":"receiver","type":"address","indexed":true},{"name":"value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"Approval","inputs":[{"name":"owner","type":"address","indexed":true},{"name":"spender","type":"address","indexed":true},{"name":"value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"TokenExchange","inputs":[{"name":"buyer","type":"address","indexed":true},{"name":"sold_id","type":"int128","indexed":false},{"name":"tokens_sold","type":"uint256","indexed":false},{"name":"bought_id","type":"int128","indexed":false},{"name":"tokens_bought","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"TokenExchangeUnderlying","inputs":[{"name":"buyer","type":"address","indexed":true},{"name":"sold_id","type":"int128","indexed":false},{"name":"tokens_sold","type":"uint256","indexed":false},{"name":"bought_id","type":"int128","indexed":false},{"name":"tokens_bought","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"AddLiquidity","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amounts","type":"uint256[2]","indexed":false},{"name":"fees","type":"uint256[2]","indexed":false},{"name":"invariant","type":"uint256","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RemoveLiquidity","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amounts","type":"uint256[2]","indexed":false},{"name":"fees","type":"uint256[2]","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RemoveLiquidityOne","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amount","type":"uint256","indexed":false},{"name":"coin_amount","type":"uint256","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RemoveLiquidityImbalance","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"token_amounts","type":"uint256[2]","indexed":false},{"name":"fees","type":"uint256[2]","indexed":false},{"name":"invariant","type":"uint256","indexed":false},{"name":"token_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"RampA","inputs":[{"name":"old_A","type":"uint256","indexed":false},{"name":"new_A","type":"uint256","indexed":false},{"name":"initial_time","type":"uint256","indexed":false},{"name":"future_time","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"StopRampA","inputs":[{"name":"A","type":"uint256","indexed":false},{"name":"t","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"stateMutability":"nonpayable","type":"constructor","inputs":[],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"initialize","inputs":[{"name":"_name","type":"string"},{"name":"_symbol","type":"string"},{"name":"_coin","type":"address"},{"name":"_rate_multiplier","type":"uint256"},{"name":"_A","type":"uint256"},{"name":"_fee","type":"uint256"}],"outputs":[],"gas":491073},{"stateMutability":"view","type":"function","name":"decimals","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":390},{"stateMutability":"nonpayable","type":"function","name":"transfer","inputs":[{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":79005},{"stateMutability":"nonpayable","type":"function","name":"transferFrom","inputs":[{"name":"_from","type":"address"},{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":116985},{"stateMutability":"nonpayable","type":"function","name":"approve","inputs":[{"name":"_spender","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":39211},{"stateMutability":"nonpayable","type":"function","name":"permit","inputs":[{"name":"_owner","type":"address"},{"name":"_spender","type":"address"},{"name":"_value","type":"uint256"},{"name":"_deadline","type":"uint256"},{"name":"_v","type":"uint8"},{"name":"_r","type":"bytes32"},{"name":"_s","type":"bytes32"}],"outputs":[{"name":"","type":"bool"}],"gas":102281},{"stateMutability":"view","type":"function","name":"admin_fee","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":540},{"stateMutability":"view","type":"function","name":"A","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":10448},{"stateMutability":"view","type":"function","name":"A_precise","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":10448},{"stateMutability":"view","type":"function","name":"get_virtual_price","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":807920},{"stateMutability":"view","type":"function","name":"calc_token_amount","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_is_deposit","type":"bool"}],"outputs":[{"name":"","type":"uint256"}],"gas":1597346},{"stateMutability":"nonpayable","type":"function","name":"add_liquidity","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_min_mint_amount","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":2611832},{"stateMutability":"nonpayable","type":"function","name":"add_liquidity","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_min_mint_amount","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":2611832},{"stateMutability":"view","type":"function","name":"get_dy","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"dx","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":1154525},{"stateMutability":"view","type":"function","name":"get_dy_underlying","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"dx","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":1162775},{"stateMutability":"nonpayable","type":"function","name":"exchange","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":1300799},{"stateMutability":"nonpayable","type":"function","name":"exchange","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":1300799},{"stateMutability":"nonpayable","type":"function","name":"exchange_underlying","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":1323223},{"stateMutability":"nonpayable","type":"function","name":"exchange_underlying","inputs":[{"name":"i","type":"int128"},{"name":"j","type":"int128"},{"name":"_dx","type":"uint256"},{"name":"_min_dy","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":1323223},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"_min_amounts","type":"uint256[2]"}],"outputs":[{"name":"","type":"uint256[2]"}],"gas":229848},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"_min_amounts","type":"uint256[2]"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256[2]"}],"gas":229848},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_imbalance","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_max_burn_amount","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":2612120},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_imbalance","inputs":[{"name":"_amounts","type":"uint256[2]"},{"name":"_max_burn_amount","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":2612120},{"stateMutability":"view","type":"function","name":"calc_withdraw_one_coin","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"i","type":"int128"}],"outputs":[{"name":"","type":"uint256"}],"gas":1259},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_one_coin","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"i","type":"int128"},{"name":"_min_received","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":1688189},{"stateMutability":"nonpayable","type":"function","name":"remove_liquidity_one_coin","inputs":[{"name":"_burn_amount","type":"uint256"},{"name":"i","type":"int128"},{"name":"_min_received","type":"uint256"},{"name":"_receiver","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":1688189},{"stateMutability":"nonpayable","type":"function","name":"ramp_A","inputs":[{"name":"_future_A","type":"uint256"},{"name":"_future_time","type":"uint256"}],"outputs":[],"gas":161164},{"stateMutability":"nonpayable","type":"function","name":"stop_ramp_A","inputs":[],"outputs":[],"gas":157387},{"stateMutability":"view","type":"function","name":"admin_balances","inputs":[{"name":"i","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":7859},{"stateMutability":"nonpayable","type":"function","name":"withdraw_admin_fees","inputs":[],"outputs":[],"gas":31294},{"stateMutability":"view","type":"function","name":"version","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":6707},{"stateMutability":"view","type":"function","name":"coins","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"address"}],"gas":3255},{"stateMutability":"view","type":"function","name":"balances","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":3285},{"stateMutability":"view","type":"function","name":"fee","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3270},{"stateMutability":"view","type":"function","name":"initial_A","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3300},{"stateMutability":"view","type":"function","name":"future_A","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3330},{"stateMutability":"view","type":"function","name":"initial_A_time","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3360},{"stateMutability":"view","type":"function","name":"future_A_time","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3390},{"stateMutability":"view","type":"function","name":"name","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":13709},{"stateMutability":"view","type":"function","name":"symbol","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":11468},{"stateMutability":"view","type":"function","name":"balanceOf","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3746},{"stateMutability":"view","type":"function","name":"allowance","inputs":[{"name":"arg0","type":"address"},{"name":"arg1","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":4042},{"stateMutability":"view","type":"function","name":"totalSupply","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3540},{"stateMutability":"view","type":"function","name":"DOMAIN_SEPARATOR","inputs":[],"outputs":[{"name":"","type":"bytes32"}],"gas":3570},{"stateMutability":"view","type":"function","name":"nonces","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3866}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dolafraxbp_pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOLAFRAXBP Gauge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xbe266d68ce3ddfab366bb866f4353b6fc42ba43c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"name":"Deposit","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"Withdraw","inputs":[{"name":"provider","type":"address","indexed":true},{"name":"value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"UpdateLiquidityLimit","inputs":[{"name":"user","type":"address","indexed":false},{"name":"original_balance","type":"uint256","indexed":false},{"name":"original_supply","type":"uint256","indexed":false},{"name":"working_balance","type":"uint256","indexed":false},{"name":"working_supply","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"CommitOwnership","inputs":[{"name":"admin","type":"address","indexed":false}],"anonymous":false,"type":"event"},{"name":"ApplyOwnership","inputs":[{"name":"admin","type":"address","indexed":false}],"anonymous":false,"type":"event"},{"name":"Transfer","inputs":[{"name":"_from","type":"address","indexed":true},{"name":"_to","type":"address","indexed":true},{"name":"_value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"name":"Approval","inputs":[{"name":"_owner","type":"address","indexed":true},{"name":"_spender","type":"address","indexed":true},{"name":"_value","type":"uint256","indexed":false}],"anonymous":false,"type":"event"},{"stateMutability":"nonpayable","type":"constructor","inputs":[],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"initialize","inputs":[{"name":"_lp_token","type":"address"}],"outputs":[],"gas":374587},{"stateMutability":"view","type":"function","name":"decimals","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":318},{"stateMutability":"view","type":"function","name":"integrate_checkpoint","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":4590},{"stateMutability":"nonpayable","type":"function","name":"user_checkpoint","inputs":[{"name":"addr","type":"address"}],"outputs":[{"name":"","type":"bool"}],"gas":3123886},{"stateMutability":"nonpayable","type":"function","name":"claimable_tokens","inputs":[{"name":"addr","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3038676},{"stateMutability":"view","type":"function","name":"claimed_reward","inputs":[{"name":"_addr","type":"address"},{"name":"_token","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3036},{"stateMutability":"view","type":"function","name":"claimable_reward","inputs":[{"name":"_user","type":"address"},{"name":"_reward_token","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":20255},{"stateMutability":"nonpayable","type":"function","name":"set_rewards_receiver","inputs":[{"name":"_receiver","type":"address"}],"outputs":[],"gas":35673},{"stateMutability":"nonpayable","type":"function","name":"claim_rewards","inputs":[],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"claim_rewards","inputs":[{"name":"_addr","type":"address"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"claim_rewards","inputs":[{"name":"_addr","type":"address"},{"name":"_receiver","type":"address"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"kick","inputs":[{"name":"addr","type":"address"}],"outputs":[],"gas":3137977},{"stateMutability":"nonpayable","type":"function","name":"deposit","inputs":[{"name":"_value","type":"uint256"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"deposit","inputs":[{"name":"_value","type":"uint256"},{"name":"_addr","type":"address"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"deposit","inputs":[{"name":"_value","type":"uint256"},{"name":"_addr","type":"address"},{"name":"_claim_rewards","type":"bool"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"withdraw","inputs":[{"name":"_value","type":"uint256"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"withdraw","inputs":[{"name":"_value","type":"uint256"},{"name":"_claim_rewards","type":"bool"}],"outputs":[]},{"stateMutability":"nonpayable","type":"function","name":"transfer","inputs":[{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":18062826},{"stateMutability":"nonpayable","type":"function","name":"transferFrom","inputs":[{"name":"_from","type":"address"},{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":18100776},{"stateMutability":"nonpayable","type":"function","name":"approve","inputs":[{"name":"_spender","type":"address"},{"name":"_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":38151},{"stateMutability":"nonpayable","type":"function","name":"increaseAllowance","inputs":[{"name":"_spender","type":"address"},{"name":"_added_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":40695},{"stateMutability":"nonpayable","type":"function","name":"decreaseAllowance","inputs":[{"name":"_spender","type":"address"},{"name":"_subtracted_value","type":"uint256"}],"outputs":[{"name":"","type":"bool"}],"gas":40719},{"stateMutability":"nonpayable","type":"function","name":"add_reward","inputs":[{"name":"_reward_token","type":"address"},{"name":"_distributor","type":"address"}],"outputs":[],"gas":115414},{"stateMutability":"nonpayable","type":"function","name":"set_reward_distributor","inputs":[{"name":"_reward_token","type":"address"},{"name":"_distributor","type":"address"}],"outputs":[],"gas":43179},{"stateMutability":"nonpayable","type":"function","name":"deposit_reward_token","inputs":[{"name":"_reward_token","type":"address"},{"name":"_amount","type":"uint256"}],"outputs":[],"gas":1540067},{"stateMutability":"nonpayable","type":"function","name":"set_killed","inputs":[{"name":"_is_killed","type":"bool"}],"outputs":[],"gas":40529},{"stateMutability":"view","type":"function","name":"lp_token","inputs":[],"outputs":[{"name":"","type":"address"}],"gas":3018},{"stateMutability":"view","type":"function","name":"future_epoch_time","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3048},{"stateMutability":"view","type":"function","name":"balanceOf","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3293},{"stateMutability":"view","type":"function","name":"totalSupply","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3108},{"stateMutability":"view","type":"function","name":"allowance","inputs":[{"name":"arg0","type":"address"},{"name":"arg1","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3568},{"stateMutability":"view","type":"function","name":"name","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":13398},{"stateMutability":"view","type":"function","name":"symbol","inputs":[],"outputs":[{"name":"","type":"string"}],"gas":11151},{"stateMutability":"view","type":"function","name":"working_balances","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3443},{"stateMutability":"view","type":"function","name":"working_supply","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3258},{"stateMutability":"view","type":"function","name":"period","inputs":[],"outputs":[{"name":"","type":"int128"}],"gas":3288},{"stateMutability":"view","type":"function","name":"period_timestamp","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":3363},{"stateMutability":"view","type":"function","name":"integrate_inv_supply","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"uint256"}],"gas":3393},{"stateMutability":"view","type":"function","name":"integrate_inv_supply_of","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3593},{"stateMutability":"view","type":"function","name":"integrate_checkpoint_of","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3623},{"stateMutability":"view","type":"function","name":"integrate_fraction","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":3653},{"stateMutability":"view","type":"function","name":"inflation_rate","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3468},{"stateMutability":"view","type":"function","name":"reward_count","inputs":[],"outputs":[{"name":"","type":"uint256"}],"gas":3498},{"stateMutability":"view","type":"function","name":"reward_tokens","inputs":[{"name":"arg0","type":"uint256"}],"outputs":[{"name":"","type":"address"}],"gas":3573},{"stateMutability":"view","type":"function","name":"reward_data","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"token","type":"address"},{"name":"distributor","type":"address"},{"name":"period_finish","type":"uint256"},{"name":"rate","type":"uint256"},{"name":"last_update","type":"uint256"},{"name":"integral","type":"uint256"}],"gas":15003},{"stateMutability":"view","type":"function","name":"rewards_receiver","inputs":[{"name":"arg0","type":"address"}],"outputs":[{"name":"","type":"address"}],"gas":3803},{"stateMutability":"view","type":"function","name":"reward_integral_for","inputs":[{"name":"arg0","type":"address"},{"name":"arg1","type":"address"}],"outputs":[{"name":"","type":"uint256"}],"gas":4048},{"stateMutability":"view","type":"function","name":"is_killed","inputs":[],"outputs":[{"name":"","type":"bool"}],"gas":3648},{"stateMutability":"view","type":"function","name":"factory","inputs":[],"outputs":[{"name":"","type":"address"}],"gas":3678}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curve Gauge Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2F50D538606Fa9EDD2B11E2446BEb18C9D5846bB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"name":"CommitOwnership","inputs":[{"type":"address","name":"admin","indexed":false}],"anonymous":false,"type":"event"},{"name":"ApplyOwnership","inputs":[{"type":"address","name":"admin","indexed":false}],"anonymous":false,"type":"event"},{"name":"AddType","inputs":[{"type":"string","name":"name","indexed":false},{"type":"int128","name":"type_id","indexed":false}],"anonymous":false,"type":"event"},{"name":"NewTypeWeight","inputs":[{"type":"int128","name":"type_id","indexed":false},{"type":"uint256","name":"time","indexed":false},{"type":"uint256","name":"weight","indexed":false},{"type":"uint256","name":"total_weight","indexed":false}],"anonymous":false,"type":"event"},{"name":"NewGaugeWeight","inputs":[{"type":"address","name":"gauge_address","indexed":false},{"type":"uint256","name":"time","indexed":false},{"type":"uint256","name":"weight","indexed":false},{"type":"uint256","name":"total_weight","indexed":false}],"anonymous":false,"type":"event"},{"name":"VoteForGauge","inputs":[{"type":"uint256","name":"time","indexed":false},{"type":"address","name":"user","indexed":false},{"type":"address","name":"gauge_addr","indexed":false},{"type":"uint256","name":"weight","indexed":false}],"anonymous":false,"type":"event"},{"name":"NewGauge","inputs":[{"type":"address","name":"addr","indexed":false},{"type":"int128","name":"gauge_type","indexed":false},{"type":"uint256","name":"weight","indexed":false}],"anonymous":false,"type":"event"},{"outputs":[],"inputs":[{"type":"address","name":"_token"},{"type":"address","name":"_voting_escrow"}],"stateMutability":"nonpayable","type":"constructor"},{"name":"commit_transfer_ownership","outputs":[],"inputs":[{"type":"address","name":"addr"}],"stateMutability":"nonpayable","type":"function","gas":37597},{"name":"apply_transfer_ownership","outputs":[],"inputs":[],"stateMutability":"nonpayable","type":"function","gas":38497},{"name":"gauge_types","outputs":[{"type":"int128","name":""}],"inputs":[{"type":"address","name":"_addr"}],"stateMutability":"view","type":"function","gas":1625},{"name":"add_gauge","outputs":[],"inputs":[{"type":"address","name":"addr"},{"type":"int128","name":"gauge_type"}],"stateMutability":"nonpayable","type":"function"},{"name":"add_gauge","outputs":[],"inputs":[{"type":"address","name":"addr"},{"type":"int128","name":"gauge_type"},{"type":"uint256","name":"weight"}],"stateMutability":"nonpayable","type":"function"},{"name":"checkpoint","outputs":[],"inputs":[],"stateMutability":"nonpayable","type":"function","gas":18033784416},{"name":"checkpoint_gauge","outputs":[],"inputs":[{"type":"address","name":"addr"}],"stateMutability":"nonpayable","type":"function","gas":18087678795},{"name":"gauge_relative_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"addr"}],"stateMutability":"view","type":"function"},{"name":"gauge_relative_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"addr"},{"type":"uint256","name":"time"}],"stateMutability":"view","type":"function"},{"name":"gauge_relative_weight_write","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"addr"}],"stateMutability":"nonpayable","type":"function"},{"name":"gauge_relative_weight_write","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"addr"},{"type":"uint256","name":"time"}],"stateMutability":"nonpayable","type":"function"},{"name":"add_type","outputs":[],"inputs":[{"type":"string","name":"_name"}],"stateMutability":"nonpayable","type":"function"},{"name":"add_type","outputs":[],"inputs":[{"type":"string","name":"_name"},{"type":"uint256","name":"weight"}],"stateMutability":"nonpayable","type":"function"},{"name":"change_type_weight","outputs":[],"inputs":[{"type":"int128","name":"type_id"},{"type":"uint256","name":"weight"}],"stateMutability":"nonpayable","type":"function","gas":36246310050},{"name":"change_gauge_weight","outputs":[],"inputs":[{"type":"address","name":"addr"},{"type":"uint256","name":"weight"}],"stateMutability":"nonpayable","type":"function","gas":36354170809},{"name":"vote_for_gauge_weights","outputs":[],"inputs":[{"type":"address","name":"_gauge_addr"},{"type":"uint256","name":"_user_weight"}],"stateMutability":"nonpayable","type":"function","gas":18142052127},{"name":"get_gauge_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"addr"}],"stateMutability":"view","type":"function","gas":2974},{"name":"get_type_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"int128","name":"type_id"}],"stateMutability":"view","type":"function","gas":2977},{"name":"get_total_weight","outputs":[{"type":"uint256","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":2693},{"name":"get_weights_sum_per_type","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"int128","name":"type_id"}],"stateMutability":"view","type":"function","gas":3109},{"name":"admin","outputs":[{"type":"address","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":1841},{"name":"future_admin","outputs":[{"type":"address","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":1871},{"name":"token","outputs":[{"type":"address","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":1901},{"name":"voting_escrow","outputs":[{"type":"address","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":1931},{"name":"n_gauge_types","outputs":[{"type":"int128","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":1961},{"name":"n_gauges","outputs":[{"type":"int128","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":1991},{"name":"gauge_type_names","outputs":[{"type":"string","name":""}],"inputs":[{"type":"int128","name":"arg0"}],"stateMutability":"view","type":"function","gas":8628},{"name":"gauges","outputs":[{"type":"address","name":""}],"inputs":[{"type":"uint256","name":"arg0"}],"stateMutability":"view","type":"function","gas":2160},{"name":"vote_user_slopes","outputs":[{"type":"uint256","name":"slope"},{"type":"uint256","name":"power"},{"type":"uint256","name":"end"}],"inputs":[{"type":"address","name":"arg0"},{"type":"address","name":"arg1"}],"stateMutability":"view","type":"function","gas":5020},{"name":"vote_user_power","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"arg0"}],"stateMutability":"view","type":"function","gas":2265},{"name":"last_user_vote","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"arg0"},{"type":"address","name":"arg1"}],"stateMutability":"view","type":"function","gas":2449},{"name":"points_weight","outputs":[{"type":"uint256","name":"bias"},{"type":"uint256","name":"slope"}],"inputs":[{"type":"address","name":"arg0"},{"type":"uint256","name":"arg1"}],"stateMutability":"view","type":"function","gas":3859},{"name":"time_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"address","name":"arg0"}],"stateMutability":"view","type":"function","gas":2355},{"name":"points_sum","outputs":[{"type":"uint256","name":"bias"},{"type":"uint256","name":"slope"}],"inputs":[{"type":"int128","name":"arg0"},{"type":"uint256","name":"arg1"}],"stateMutability":"view","type":"function","gas":3970},{"name":"time_sum","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"uint256","name":"arg0"}],"stateMutability":"view","type":"function","gas":2370},{"name":"points_total","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"uint256","name":"arg0"}],"stateMutability":"view","type":"function","gas":2406},{"name":"time_total","outputs":[{"type":"uint256","name":""}],"inputs":[],"stateMutability":"view","type":"function","gas":2321},{"name":"points_type_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"int128","name":"arg0"},{"type":"uint256","name":"arg1"}],"stateMutability":"view","type":"function","gas":2671},{"name":"time_type_weight","outputs":[{"type":"uint256","name":""}],"inputs":[{"type":"uint256","name":"arg0"}],"stateMutability":"view","type":"function","gas":2490}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dolafraxbp_gauge</t>
   </si>
   <si>
     <t xml:space="preserve">lending2</t>
@@ -1900,7 +1934,7 @@
     <cellStyle name="Excel Built-in Good" xfId="22"/>
     <cellStyle name="Excel Built-in Calculation" xfId="23"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1934,6 +1968,69 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFDDE8CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006100"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9C0006"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9C6500"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA7D00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2005,6 +2102,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2013,8 +2114,8 @@
   </sheetPr>
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E44" activeCellId="1" sqref="D:D E44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2946,6 +3047,66 @@
         <v>120</v>
       </c>
       <c r="F46" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2978,10 +3139,10 @@
     <tabColor rgb="FFDDE8CB"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="1" sqref="D:D J3"/>
+      <selection pane="topLeft" activeCell="K14" activeCellId="1" sqref="D48 K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2990,6 +3151,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -3004,10 +3166,10 @@
         <v>37</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>19</v>
@@ -3024,93 +3186,111 @@
       <c r="J1" s="11" t="s">
         <v>117</v>
       </c>
+      <c r="K1" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>136</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
+      <c r="K3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="L3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
+      <c r="K4" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -3120,10 +3300,12 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -3134,10 +3316,12 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -3148,6 +3332,8 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
@@ -3160,6 +3346,8 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3180,8 +3368,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="D48 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3205,16 +3393,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3279,7 +3467,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="D:D B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="D48 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3344,19 +3532,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <tabColor rgb="FFFFE994"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H69" activeCellId="1" sqref="D:D H69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A150" activeCellId="1" sqref="D48 A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3367,36 +3556,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>61</v>
@@ -3406,7 +3595,7 @@
         <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sync","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>79</v>
       </c>
@@ -3414,10 +3603,10 @@
         <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>77</v>
@@ -3427,322 +3616,322 @@
         <v>[{"inputs":[{"internalType":"address","name":"_singleton","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"stateMutability":"payable","type":"fallback"}]</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">IF(F4="",E4,G4)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H5" s="0" t="str">
         <f aca="false">IF(F5="",E5,G5)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>164</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H6" s="0" t="str">
         <f aca="false">IF(F6="",E6,G6)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H7" s="0" t="str">
         <f aca="false">IF(F7="",E7,G7)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>169</v>
       </c>
       <c r="H8" s="0" t="str">
         <f aca="false">IF(F8="",E8,G8)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H9" s="0" t="str">
         <f aca="false">IF(F9="",E9,G9)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H10" s="0" t="str">
         <f aca="false">IF(F10="",E10,G10)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H11" s="0" t="str">
         <f aca="false">IF(F11="",E11,G11)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">IF(F12="",E12,G12)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H13" s="0" t="str">
         <f aca="false">IF(F13="",E13,G13)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H14" s="0" t="str">
         <f aca="false">IF(F14="",E14,G14)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">IF(F15="",E15,G15)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1In","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount0Out","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1Out","type":"uint256"},{"indexed":true,"internalType":"address","name":"to","type":"address"}],"name":"Swap","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint112","name":"reserve0","type":"uint112"},{"indexed":false,"internalType":"uint112","name":"reserve1","type":"uint112"}],"name":"Sync","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":true,"inputs":[],"name":"DOMAIN_SEPARATOR","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"MINIMUM_LIQUIDITY","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"PERMIT_TYPEHASH","outputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"address","name":"","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getReserves","outputs":[{"internalType":"uint112","name":"_reserve0","type":"uint112"},{"internalType":"uint112","name":"_reserve1","type":"uint112"},{"internalType":"uint32","name":"_blockTimestampLast","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_token0","type":"address"},{"internalType":"address","name":"_token1","type":"address"}],"name":"initialize","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"kLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"mint","outputs":[{"internalType":"uint256","name":"liquidity","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"nonces","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"},{"internalType":"uint256","name":"deadline","type":"uint256"},{"internalType":"uint8","name":"v","type":"uint8"},{"internalType":"bytes32","name":"r","type":"bytes32"},{"internalType":"bytes32","name":"s","type":"bytes32"}],"name":"permit","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"price0CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"price1CumulativeLast","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"}],"name":"skim","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"amount0Out","type":"uint256"},{"internalType":"uint256","name":"amount1Out","type":"uint256"},{"internalType":"address","name":"to","type":"address"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"sync","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"from","type":"address"},{"internalType":"address","name":"to","type":"address"},{"internalType":"uint256","name":"value","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">IF(F16="",E16,G16)</f>
         <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount","type":"uint128"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":false,"internalType":"address","name":"recipient","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount0","type":"uint128"},{"indexed":false,"internalType":"uint128","name":"amount1","type":"uint128"}],"name":"Collect","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint128","name":"amount0","type":"uint128"},{"indexed":false,"internalType":"uint128","name":"amount1","type":"uint128"}],"name":"CollectProtocol","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paid0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paid1","type":"uint256"}],"name":"Flash","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint16","name":"observationCardinalityNextOld","type":"uint16"},{"indexed":false,"internalType":"uint16","name":"observationCardinalityNextNew","type":"uint16"}],"name":"IncreaseObservationCardinalityNext","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"indexed":false,"internalType":"int24","name":"tick","type":"int24"}],"name":"Initialize","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount","type":"uint128"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint8","name":"feeProtocol0Old","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol1Old","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol0New","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol1New","type":"uint8"}],"name":"SetFeeProtocol","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"int256","name":"amount0","type":"int256"},{"indexed":false,"internalType":"int256","name":"amount1","type":"int256"},{"indexed":false,"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"indexed":false,"internalType":"uint128","name":"liquidity","type":"uint128"},{"indexed":false,"internalType":"int24","name":"tick","type":"int24"}],"name":"Swap","type":"event"},{"inputs":[{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount","type":"uint128"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount0Requested","type":"uint128"},{"internalType":"uint128","name":"amount1Requested","type":"uint128"}],"name":"collect","outputs":[{"internalType":"uint128","name":"amount0","type":"uint128"},{"internalType":"uint128","name":"amount1","type":"uint128"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint128","name":"amount0Requested","type":"uint128"},{"internalType":"uint128","name":"amount1Requested","type":"uint128"}],"name":"collectProtocol","outputs":[{"internalType":"uint128","name":"amount0","type":"uint128"},{"internalType":"uint128","name":"amount1","type":"uint128"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"fee","outputs":[{"internalType":"uint24","name":"","type":"uint24"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeGrowthGlobal0X128","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeGrowthGlobal1X128","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"flash","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint16","name":"observationCardinalityNext","type":"uint16"}],"name":"increaseObservationCardinalityNext","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"liquidity","outputs":[{"internalType":"uint128","name":"","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxLiquidityPerTick","outputs":[{"internalType":"uint128","name":"","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount","type":"uint128"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"mint","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"observations","outputs":[{"internalType":"uint32","name":"blockTimestamp","type":"uint32"},{"internalType":"int56","name":"tickCumulative","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityCumulativeX128","type":"uint160"},{"internalType":"bool","name":"initialized","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint32[]","name":"secondsAgos","type":"uint32[]"}],"name":"observe","outputs":[{"internalType":"int56[]","name":"tickCumulatives","type":"int56[]"},{"internalType":"uint160[]","name":"secondsPerLiquidityCumulativeX128s","type":"uint160[]"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"name":"positions","outputs":[{"internalType":"uint128","name":"liquidity","type":"uint128"},{"internalType":"uint256","name":"feeGrowthInside0LastX128","type":"uint256"},{"internalType":"uint256","name":"feeGrowthInside1LastX128","type":"uint256"},{"internalType":"uint128","name":"tokensOwed0","type":"uint128"},{"internalType":"uint128","name":"tokensOwed1","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"protocolFees","outputs":[{"internalType":"uint128","name":"token0","type":"uint128"},{"internalType":"uint128","name":"token1","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint8","name":"feeProtocol0","type":"uint8"},{"internalType":"uint8","name":"feeProtocol1","type":"uint8"}],"name":"setFeeProtocol","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"slot0","outputs":[{"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"internalType":"int24","name":"tick","type":"int24"},{"internalType":"uint16","name":"observationIndex","type":"uint16"},{"internalType":"uint16","name":"observationCardinality","type":"uint16"},{"internalType":"uint16","name":"observationCardinalityNext","type":"uint16"},{"internalType":"uint8","name":"feeProtocol","type":"uint8"},{"internalType":"bool","name":"unlocked","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"}],"name":"snapshotCumulativesInside","outputs":[{"internalType":"int56","name":"tickCumulativeInside","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityInsideX128","type":"uint160"},{"internalType":"uint32","name":"secondsInside","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"bool","name":"zeroForOne","type":"bool"},{"internalType":"int256","name":"amountSpecified","type":"int256"},{"internalType":"uint160","name":"sqrtPriceLimitX96","type":"uint160"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[{"internalType":"int256","name":"amount0","type":"int256"},{"internalType":"int256","name":"amount1","type":"int256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"int16","name":"","type":"int16"}],"name":"tickBitmap","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"tickSpacing","outputs":[{"internalType":"int24","name":"","type":"int24"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"int24","name":"","type":"int24"}],"name":"ticks","outputs":[{"internalType":"uint128","name":"liquidityGross","type":"uint128"},{"internalType":"int128","name":"liquidityNet","type":"int128"},{"internalType":"uint256","name":"feeGrowthOutside0X128","type":"uint256"},{"internalType":"uint256","name":"feeGrowthOutside1X128","type":"uint256"},{"internalType":"int56","name":"tickCumulativeOutside","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityOutsideX128","type":"uint160"},{"internalType":"uint32","name":"secondsOutside","type":"uint32"},{"internalType":"bool","name":"initialized","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"}]</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">IF(F17="",E17,G17)</f>
         <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount","type":"uint128"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":false,"internalType":"address","name":"recipient","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount0","type":"uint128"},{"indexed":false,"internalType":"uint128","name":"amount1","type":"uint128"}],"name":"Collect","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint128","name":"amount0","type":"uint128"},{"indexed":false,"internalType":"uint128","name":"amount1","type":"uint128"}],"name":"CollectProtocol","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paid0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paid1","type":"uint256"}],"name":"Flash","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint16","name":"observationCardinalityNextOld","type":"uint16"},{"indexed":false,"internalType":"uint16","name":"observationCardinalityNextNew","type":"uint16"}],"name":"IncreaseObservationCardinalityNext","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"indexed":false,"internalType":"int24","name":"tick","type":"int24"}],"name":"Initialize","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount","type":"uint128"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint8","name":"feeProtocol0Old","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol1Old","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol0New","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol1New","type":"uint8"}],"name":"SetFeeProtocol","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"int256","name":"amount0","type":"int256"},{"indexed":false,"internalType":"int256","name":"amount1","type":"int256"},{"indexed":false,"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"indexed":false,"internalType":"uint128","name":"liquidity","type":"uint128"},{"indexed":false,"internalType":"int24","name":"tick","type":"int24"}],"name":"Swap","type":"event"},{"inputs":[{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount","type":"uint128"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount0Requested","type":"uint128"},{"internalType":"uint128","name":"amount1Requested","type":"uint128"}],"name":"collect","outputs":[{"internalType":"uint128","name":"amount0","type":"uint128"},{"internalType":"uint128","name":"amount1","type":"uint128"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint128","name":"amount0Requested","type":"uint128"},{"internalType":"uint128","name":"amount1Requested","type":"uint128"}],"name":"collectProtocol","outputs":[{"internalType":"uint128","name":"amount0","type":"uint128"},{"internalType":"uint128","name":"amount1","type":"uint128"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"fee","outputs":[{"internalType":"uint24","name":"","type":"uint24"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeGrowthGlobal0X128","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeGrowthGlobal1X128","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"flash","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint16","name":"observationCardinalityNext","type":"uint16"}],"name":"increaseObservationCardinalityNext","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"liquidity","outputs":[{"internalType":"uint128","name":"","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxLiquidityPerTick","outputs":[{"internalType":"uint128","name":"","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount","type":"uint128"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"mint","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"observations","outputs":[{"internalType":"uint32","name":"blockTimestamp","type":"uint32"},{"internalType":"int56","name":"tickCumulative","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityCumulativeX128","type":"uint160"},{"internalType":"bool","name":"initialized","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint32[]","name":"secondsAgos","type":"uint32[]"}],"name":"observe","outputs":[{"internalType":"int56[]","name":"tickCumulatives","type":"int56[]"},{"internalType":"uint160[]","name":"secondsPerLiquidityCumulativeX128s","type":"uint160[]"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"name":"positions","outputs":[{"internalType":"uint128","name":"liquidity","type":"uint128"},{"internalType":"uint256","name":"feeGrowthInside0LastX128","type":"uint256"},{"internalType":"uint256","name":"feeGrowthInside1LastX128","type":"uint256"},{"internalType":"uint128","name":"tokensOwed0","type":"uint128"},{"internalType":"uint128","name":"tokensOwed1","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"protocolFees","outputs":[{"internalType":"uint128","name":"token0","type":"uint128"},{"internalType":"uint128","name":"token1","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint8","name":"feeProtocol0","type":"uint8"},{"internalType":"uint8","name":"feeProtocol1","type":"uint8"}],"name":"setFeeProtocol","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"slot0","outputs":[{"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"internalType":"int24","name":"tick","type":"int24"},{"internalType":"uint16","name":"observationIndex","type":"uint16"},{"internalType":"uint16","name":"observationCardinality","type":"uint16"},{"internalType":"uint16","name":"observationCardinalityNext","type":"uint16"},{"internalType":"uint8","name":"feeProtocol","type":"uint8"},{"internalType":"bool","name":"unlocked","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"}],"name":"snapshotCumulativesInside","outputs":[{"internalType":"int56","name":"tickCumulativeInside","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityInsideX128","type":"uint160"},{"internalType":"uint32","name":"secondsInside","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"bool","name":"zeroForOne","type":"bool"},{"internalType":"int256","name":"amountSpecified","type":"int256"},{"internalType":"uint160","name":"sqrtPriceLimitX96","type":"uint160"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[{"internalType":"int256","name":"amount0","type":"int256"},{"internalType":"int256","name":"amount1","type":"int256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"int16","name":"","type":"int16"}],"name":"tickBitmap","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"tickSpacing","outputs":[{"internalType":"int24","name":"","type":"int24"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"int24","name":"","type":"int24"}],"name":"ticks","outputs":[{"internalType":"uint128","name":"liquidityGross","type":"uint128"},{"internalType":"int128","name":"liquidityNet","type":"int128"},{"internalType":"uint256","name":"feeGrowthOutside0X128","type":"uint256"},{"internalType":"uint256","name":"feeGrowthOutside1X128","type":"uint256"},{"internalType":"int56","name":"tickCumulativeOutside","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityOutsideX128","type":"uint160"},{"internalType":"uint32","name":"secondsOutside","type":"uint32"},{"internalType":"bool","name":"initialized","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"}]</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">IF(F18="",E18,G18)</f>
         <v>[{"inputs":[],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount","type":"uint128"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":false,"internalType":"address","name":"recipient","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount0","type":"uint128"},{"indexed":false,"internalType":"uint128","name":"amount1","type":"uint128"}],"name":"Collect","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint128","name":"amount0","type":"uint128"},{"indexed":false,"internalType":"uint128","name":"amount1","type":"uint128"}],"name":"CollectProtocol","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paid0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"paid1","type":"uint256"}],"name":"Flash","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint16","name":"observationCardinalityNextOld","type":"uint16"},{"indexed":false,"internalType":"uint16","name":"observationCardinalityNextNew","type":"uint16"}],"name":"IncreaseObservationCardinalityNext","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"indexed":false,"internalType":"int24","name":"tick","type":"int24"}],"name":"Initialize","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"int24","name":"tickLower","type":"int24"},{"indexed":true,"internalType":"int24","name":"tickUpper","type":"int24"},{"indexed":false,"internalType":"uint128","name":"amount","type":"uint128"},{"indexed":false,"internalType":"uint256","name":"amount0","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"amount1","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint8","name":"feeProtocol0Old","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol1Old","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol0New","type":"uint8"},{"indexed":false,"internalType":"uint8","name":"feeProtocol1New","type":"uint8"}],"name":"SetFeeProtocol","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"sender","type":"address"},{"indexed":true,"internalType":"address","name":"recipient","type":"address"},{"indexed":false,"internalType":"int256","name":"amount0","type":"int256"},{"indexed":false,"internalType":"int256","name":"amount1","type":"int256"},{"indexed":false,"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"indexed":false,"internalType":"uint128","name":"liquidity","type":"uint128"},{"indexed":false,"internalType":"int24","name":"tick","type":"int24"}],"name":"Swap","type":"event"},{"inputs":[{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount","type":"uint128"}],"name":"burn","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount0Requested","type":"uint128"},{"internalType":"uint128","name":"amount1Requested","type":"uint128"}],"name":"collect","outputs":[{"internalType":"uint128","name":"amount0","type":"uint128"},{"internalType":"uint128","name":"amount1","type":"uint128"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint128","name":"amount0Requested","type":"uint128"},{"internalType":"uint128","name":"amount1Requested","type":"uint128"}],"name":"collectProtocol","outputs":[{"internalType":"uint128","name":"amount0","type":"uint128"},{"internalType":"uint128","name":"amount1","type":"uint128"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"factory","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"fee","outputs":[{"internalType":"uint24","name":"","type":"uint24"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeGrowthGlobal0X128","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"feeGrowthGlobal1X128","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"flash","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint16","name":"observationCardinalityNext","type":"uint16"}],"name":"increaseObservationCardinalityNext","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"}],"name":"initialize","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"liquidity","outputs":[{"internalType":"uint128","name":"","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxLiquidityPerTick","outputs":[{"internalType":"uint128","name":"","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"},{"internalType":"uint128","name":"amount","type":"uint128"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"mint","outputs":[{"internalType":"uint256","name":"amount0","type":"uint256"},{"internalType":"uint256","name":"amount1","type":"uint256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"","type":"uint256"}],"name":"observations","outputs":[{"internalType":"uint32","name":"blockTimestamp","type":"uint32"},{"internalType":"int56","name":"tickCumulative","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityCumulativeX128","type":"uint160"},{"internalType":"bool","name":"initialized","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint32[]","name":"secondsAgos","type":"uint32[]"}],"name":"observe","outputs":[{"internalType":"int56[]","name":"tickCumulatives","type":"int56[]"},{"internalType":"uint160[]","name":"secondsPerLiquidityCumulativeX128s","type":"uint160[]"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"bytes32","name":"","type":"bytes32"}],"name":"positions","outputs":[{"internalType":"uint128","name":"liquidity","type":"uint128"},{"internalType":"uint256","name":"feeGrowthInside0LastX128","type":"uint256"},{"internalType":"uint256","name":"feeGrowthInside1LastX128","type":"uint256"},{"internalType":"uint128","name":"tokensOwed0","type":"uint128"},{"internalType":"uint128","name":"tokensOwed1","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"protocolFees","outputs":[{"internalType":"uint128","name":"token0","type":"uint128"},{"internalType":"uint128","name":"token1","type":"uint128"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"uint8","name":"feeProtocol0","type":"uint8"},{"internalType":"uint8","name":"feeProtocol1","type":"uint8"}],"name":"setFeeProtocol","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"slot0","outputs":[{"internalType":"uint160","name":"sqrtPriceX96","type":"uint160"},{"internalType":"int24","name":"tick","type":"int24"},{"internalType":"uint16","name":"observationIndex","type":"uint16"},{"internalType":"uint16","name":"observationCardinality","type":"uint16"},{"internalType":"uint16","name":"observationCardinalityNext","type":"uint16"},{"internalType":"uint8","name":"feeProtocol","type":"uint8"},{"internalType":"bool","name":"unlocked","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"int24","name":"tickLower","type":"int24"},{"internalType":"int24","name":"tickUpper","type":"int24"}],"name":"snapshotCumulativesInside","outputs":[{"internalType":"int56","name":"tickCumulativeInside","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityInsideX128","type":"uint160"},{"internalType":"uint32","name":"secondsInside","type":"uint32"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"bool","name":"zeroForOne","type":"bool"},{"internalType":"int256","name":"amountSpecified","type":"int256"},{"internalType":"uint160","name":"sqrtPriceLimitX96","type":"uint160"},{"internalType":"bytes","name":"data","type":"bytes"}],"name":"swap","outputs":[{"internalType":"int256","name":"amount0","type":"int256"},{"internalType":"int256","name":"amount1","type":"int256"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"int16","name":"","type":"int16"}],"name":"tickBitmap","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"tickSpacing","outputs":[{"internalType":"int24","name":"","type":"int24"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"int24","name":"","type":"int24"}],"name":"ticks","outputs":[{"internalType":"uint128","name":"liquidityGross","type":"uint128"},{"internalType":"int128","name":"liquidityNet","type":"int128"},{"internalType":"uint256","name":"feeGrowthOutside0X128","type":"uint256"},{"internalType":"uint256","name":"feeGrowthOutside1X128","type":"uint256"},{"internalType":"int56","name":"tickCumulativeOutside","type":"int56"},{"internalType":"uint160","name":"secondsPerLiquidityOutsideX128","type":"uint160"},{"internalType":"uint32","name":"secondsOutside","type":"uint32"},{"internalType":"bool","name":"initialized","type":"bool"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token0","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"token1","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"}]</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>34</v>
       </c>
@@ -3750,10 +3939,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>36</v>
@@ -3763,132 +3952,132 @@
         <v>[{"inputs":[{"internalType":"address","name":"underlying_","type":"address"},{"internalType":"contract ComptrollerInterface","name":"comptroller_","type":"address"},{"internalType":"uint256","name":"rewardPerBlock_","type":"uint256"},{"internalType":"address","name":"rewardTreasury_","type":"address"},{"internalType":"string","name":"name_","type":"string"},{"internalType":"string","name":"symbol_","type":"string"},{"internalType":"uint8","name":"decimals_","type":"uint8"},{"internalType":"address payable","name":"admin_","type":"address"}],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegator","type":"address"},{"indexed":true,"internalType":"address","name":"fromDelegate","type":"address"},{"indexed":true,"internalType":"address","name":"toDelegate","type":"address"}],"name":"DelegateChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"delegate","type":"address"},{"indexed":false,"internalType":"uint256","name":"previousBalance","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newBalance","type":"uint256"}],"name":"DelegateVotesChanged","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"error","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"info","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"detail","type":"uint256"}],"name":"Failure","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"minter","type":"address"},{"indexed":false,"internalType":"uint256","name":"mintAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"mintTokens","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newAdmin","type":"address"}],"name":"NewAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract ComptrollerInterface","name":"oldComptroller","type":"address"},{"indexed":false,"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"NewComptroller","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldPendingAdmin","type":"address"},{"indexed":false,"internalType":"address","name":"newPendingAdmin","type":"address"}],"name":"NewPendingAdmin","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"oldRewardPerBlock","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"newRewardPerBlock","type":"uint256"}],"name":"NewRewardPerBlock","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"oldRewardTreasury","type":"address"},{"indexed":false,"internalType":"address","name":"newRewardTreasury","type":"address"}],"name":"NewRewardTreasury","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"contract TimelockEscrow","name":"oldTimelockEscrow","type":"address"},{"indexed":false,"internalType":"contract TimelockEscrow","name":"newTimelockEscrow","type":"address"}],"name":"NewTimelockEscrow","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"address","name":"redeemer","type":"address"},{"indexed":false,"internalType":"uint256","name":"redeemAmount","type":"uint256"},{"indexed":false,"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"Redeem","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[],"name":"_acceptAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract ComptrollerInterface","name":"newComptroller","type":"address"}],"name":"_setComptroller","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address payable","name":"newPendingAdmin","type":"address"}],"name":"_setPendingAdmin","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"newRewardPerBlock","type":"uint256"}],"name":"_setRewardPerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"newRewardTreasury","type":"address"}],"name":"_setRewardTreasury","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"contract TimelockEscrow","name":"newTimelockEscrow","type":"address"}],"name":"_setTimelockEscrow","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"accrualBlockNumber","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"accrueInterest","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"admin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"owner","type":"address"}],"name":"balanceOfUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"borrowIndex","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"},{"internalType":"uint32","name":"","type":"uint32"}],"name":"checkpoints","outputs":[{"internalType":"uint32","name":"fromBlock","type":"uint32"},{"internalType":"uint96","name":"votes","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"comptroller","outputs":[{"internalType":"contract ComptrollerInterface","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"delegates","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"escrow","outputs":[{"internalType":"contract TimelockEscrow","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"exchangeRateCurrent","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"exchangeRateStored","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getAccountSnapshot","outputs":[{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"},{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"getCash","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"getCurrentVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"blockNumber","type":"uint256"}],"name":"getPriorVotes","outputs":[{"internalType":"uint96","name":"","type":"uint96"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"isCToken","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"mintAmount","type":"uint256"}],"name":"mint","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"numCheckpoints","outputs":[{"internalType":"uint32","name":"","type":"uint32"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingAdmin","outputs":[{"internalType":"address payable","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemTokens","type":"uint256"}],"name":"redeem","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"uint256","name":"redeemAmount","type":"uint256"}],"name":"redeemUnderlying","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"rewardPerBlock","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"rewardTreasury","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"liquidator","type":"address"},{"internalType":"address","name":"borrower","type":"address"},{"internalType":"uint256","name":"seizeTokens","type":"uint256"}],"name":"seize","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"user","type":"address"}],"name":"syncDelegate","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"underlying","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"}]</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">IF(F20="",E20,G20)</f>
         <v>[{"inputs":[{"internalType":"contract IYearnVault","name":"vault_","type":"address"},{"internalType":"address","name":"gov_","type":"address"},{"internalType":"uint256","name":"maxLossBpContraction_","type":"uint256"},{"internalType":"uint256","name":"maxLossBpTakeProfit_","type":"uint256"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Contraction","type":"event"},{"anonymous":false,"inputs":[{"indexed":false,"internalType":"uint256","name":"amount","type":"uint256"}],"name":"Expansion","type":"event"},{"inputs":[],"name":"chair","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"newChair_","type":"address"}],"name":"changeChair","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"newGov_","type":"address"}],"name":"changeGov","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"contractAll","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amountUnderlying","type":"uint256"}],"name":"contraction","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"token","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"emergencyWithdraw","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"expansion","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"gov","outputs":[{"internalType":"address","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxLossBpContraction","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"maxLossBpTakeProfit","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"resign","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"newMaxLossBpContraction","type":"uint256"}],"name":"setMaxLossBpContraction","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"newMaxLossBpTakeProfit","type":"uint256"}],"name":"setMaxLossBpTakeProfit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"supply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"takeProfit","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"underlying","outputs":[{"internalType":"contract IERC20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"vault","outputs":[{"internalType":"contract IYearnVault","name":"","type":"address"}],"stateMutability":"view","type":"function"}]</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="H21" s="0" t="str">
         <f aca="false">IF(F21="",E21,G21)</f>
         <v>[{"constant":true,"inputs":[],"name":"mintingFinished","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"_spender","type":"address"},{"name":"_value","type":"uint256"}],"name":"approve","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"_token","type":"address"}],"name":"reclaimToken","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"_from","type":"address"},{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"name":"transferFrom","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"unpause","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"_to","type":"address"},{"name":"_amount","type":"uint256"}],"name":"mint","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"value","type":"uint256"}],"name":"burn","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"claimOwnership","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"paused","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"_spender","type":"address"},{"name":"_subtractedValue","type":"uint256"}],"name":"decreaseApproval","outputs":[{"name":"success","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"_owner","type":"address"}],"name":"balanceOf","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[],"name":"renounceOwnership","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"finishMinting","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"pause","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"owner","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"_to","type":"address"},{"name":"_value","type":"uint256"}],"name":"transfer","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"_spender","type":"address"},{"name":"_addedValue","type":"uint256"}],"name":"increaseApproval","outputs":[{"name":"success","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"name":"_owner","type":"address"},{"name":"_spender","type":"address"}],"name":"allowance","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"pendingOwner","outputs":[{"name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"newOwner","type":"address"}],"name":"transferOwnership","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"anonymous":false,"inputs":[],"name":"Pause","type":"event"},{"anonymous":false,"inputs":[],"name":"Unpause","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"burner","type":"address"},{"indexed":false,"name":"value","type":"uint256"}],"name":"Burn","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"to","type":"address"},{"indexed":false,"name":"amount","type":"uint256"}],"name":"Mint","type":"event"},{"anonymous":false,"inputs":[],"name":"MintFinished","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"previousOwner","type":"address"}],"name":"OwnershipRenounced","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"previousOwner","type":"address"},{"indexed":true,"name":"newOwner","type":"address"}],"name":"OwnershipTransferred","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"owner","type":"address"},{"indexed":true,"name":"spender","type":"address"},{"indexed":false,"name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"from","type":"address"},{"indexed":true,"name":"to","type":"address"},{"indexed":false,"name":"value","type":"uint256"}],"name":"Transfer","type":"event"}]</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">IF(F22="",E22,G22)</f>
         <v>[{"constant":true,"inputs":[],"name":"name","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"guy","type":"address"},{"name":"wad","type":"uint256"}],"name":"approve","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"src","type":"address"},{"name":"dst","type":"address"},{"name":"wad","type":"uint256"}],"name":"transferFrom","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"name":"wad","type":"uint256"}],"name":"withdraw","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[{"name":"","type":"address"}],"name":"balanceOf","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"name":"dst","type":"address"},{"name":"wad","type":"uint256"}],"name":"transfer","outputs":[{"name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[],"name":"deposit","outputs":[],"payable":true,"stateMutability":"payable","type":"function"},{"constant":true,"inputs":[{"name":"","type":"address"},{"name":"","type":"address"}],"name":"allowance","outputs":[{"name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"payable":true,"stateMutability":"payable","type":"fallback"},{"anonymous":false,"inputs":[{"indexed":true,"name":"src","type":"address"},{"indexed":true,"name":"guy","type":"address"},{"indexed":false,"name":"wad","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"src","type":"address"},{"indexed":true,"name":"dst","type":"address"},{"indexed":false,"name":"wad","type":"uint256"}],"name":"Transfer","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"dst","type":"address"},{"indexed":false,"name":"wad","type":"uint256"}],"name":"Deposit","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"name":"src","type":"address"},{"indexed":false,"name":"wad","type":"uint256"}],"name":"Withdrawal","type":"event"}]</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="H23" s="0" t="str">
         <f aca="false">IF(F23="",E23,G23)</f>
         <v>[{"inputs":[],"payable":false,"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"constant":false,"inputs":[{"internalType":"address","name":"_minter","type":"address"}],"name":"addMinter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"governance","outputs":[{"internalType":"address","name":"","type":"address"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"account","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"mint","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[{"internalType":"address","name":"","type":"address"}],"name":"minters","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_minter","type":"address"}],"name":"removeMinter","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"_governance","type":"address"}],"name":"setGovernance","outputs":[],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":true,"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":true,"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"payable":false,"stateMutability":"view","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"},{"constant":false,"inputs":[{"internalType":"address","name":"sender","type":"address"},{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"payable":false,"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>220</v>
-      </c>
       <c r="E24" s="14" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="H24" s="0" t="str">
         <f aca="false">IF(F24="",E24,G24)</f>
         <v>[{"inputs":[{"internalType":"contract IERC20","name":"_sushi","type":"address"}],"stateMutability":"nonpayable","type":"constructor"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"owner","type":"address"},{"indexed":true,"internalType":"address","name":"spender","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Approval","type":"event"},{"anonymous":false,"inputs":[{"indexed":true,"internalType":"address","name":"from","type":"address"},{"indexed":true,"internalType":"address","name":"to","type":"address"},{"indexed":false,"internalType":"uint256","name":"value","type":"uint256"}],"name":"Transfer","type":"event"},{"inputs":[{"internalType":"address","name":"owner","type":"address"},{"internalType":"address","name":"spender","type":"address"}],"name":"allowance","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"approve","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"account","type":"address"}],"name":"balanceOf","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"decimals","outputs":[{"internalType":"uint8","name":"","type":"uint8"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"subtractedValue","type":"uint256"}],"name":"decreaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_amount","type":"uint256"}],"name":"enter","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"spender","type":"address"},{"internalType":"uint256","name":"addedValue","type":"uint256"}],"name":"increaseAllowance","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"uint256","name":"_share","type":"uint256"}],"name":"leave","outputs":[],"stateMutability":"nonpayable","type":"function"},{"inputs":[],"name":"name","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"sushi","outputs":[{"internalType":"contract IERC20","name":"","type":"address"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"symbol","outputs":[{"internalType":"string","name":"","type":"string"}],"stateMutability":"view","type":"function"},{"inputs":[],"name":"totalSupply","outputs":[{"internalType":"uint256","name":"","type":"uint256"}],"stateMutability":"view","type":"function"},{"inputs":[{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transfer","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"},{"inputs":[{"internalType":"address","name":"sender","type":"address"},{"internalType":"address","name":"recipient","type":"address"},{"internalType":"uint256","name":"amount","type":"uint256"}],"name":"transferFrom","outputs":[{"internalType":"bool","name":"","type":"bool"}],"stateMutability":"nonpayable","type":"function"}]</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>104</v>
       </c>
@@ -3896,10 +4085,10 @@
         <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>106</v>
@@ -3908,7 +4097,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>75</v>
       </c>
@@ -3916,10 +4105,10 @@
         <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>77</v>
@@ -3928,7 +4117,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>16</v>
       </c>
@@ -3936,10 +4125,10 @@
         <v>17</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>18</v>
@@ -3948,7 +4137,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>67</v>
       </c>
@@ -3956,19 +4145,19 @@
         <v>68</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>39</v>
       </c>
@@ -3976,10 +4165,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>41</v>
@@ -3988,7 +4177,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>43</v>
       </c>
@@ -3996,10 +4185,10 @@
         <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>41</v>
@@ -4008,7 +4197,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>45</v>
       </c>
@@ -4016,10 +4205,10 @@
         <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>41</v>
@@ -4028,7 +4217,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>47</v>
       </c>
@@ -4036,19 +4225,19 @@
         <v>48</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>49</v>
       </c>
@@ -4056,10 +4245,10 @@
         <v>50</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>101</v>
@@ -4068,18 +4257,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>106</v>
@@ -4088,27 +4277,27 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>11</v>
       </c>
@@ -4116,10 +4305,10 @@
         <v>12</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>13</v>
@@ -4128,599 +4317,599 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="F42" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>265</v>
-      </c>
       <c r="G42" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="G43" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>266</v>
-      </c>
       <c r="H43" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>273</v>
-      </c>
       <c r="F46" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>20</v>
       </c>
@@ -4728,10 +4917,10 @@
         <v>21</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>22</v>
@@ -4740,7 +4929,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>23</v>
       </c>
@@ -4748,10 +4937,10 @@
         <v>21</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>22</v>
@@ -4760,157 +4949,157 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>69</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>118</v>
       </c>
@@ -4918,16 +5107,16 @@
         <v>119</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>69</v>
@@ -4936,7 +5125,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>121</v>
       </c>
@@ -4944,16 +5133,16 @@
         <v>122</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>69</v>
@@ -4962,24 +5151,24 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>69</v>
@@ -4988,7 +5177,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>123</v>
       </c>
@@ -4996,16 +5185,16 @@
         <v>124</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>69</v>
@@ -5014,7 +5203,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>26</v>
       </c>
@@ -5022,10 +5211,10 @@
         <v>27</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>18</v>
@@ -5034,7 +5223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>28</v>
       </c>
@@ -5042,10 +5231,10 @@
         <v>29</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>18</v>
@@ -5054,7 +5243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>30</v>
       </c>
@@ -5062,10 +5251,10 @@
         <v>31</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>18</v>
@@ -5074,7 +5263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>32</v>
       </c>
@@ -5082,10 +5271,10 @@
         <v>33</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>18</v>
@@ -5094,156 +5283,156 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>61</v>
@@ -5252,7 +5441,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>59</v>
       </c>
@@ -5260,10 +5449,10 @@
         <v>60</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>61</v>
@@ -5272,7 +5461,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>63</v>
       </c>
@@ -5280,10 +5469,10 @@
         <v>64</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>61</v>
@@ -5292,18 +5481,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>61</v>
@@ -5312,18 +5501,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>61</v>
@@ -5332,18 +5521,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>61</v>
@@ -5352,18 +5541,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>61</v>
@@ -5372,103 +5561,103 @@
         <v>61</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>102</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>77</v>
@@ -5480,15 +5669,15 @@
         <v>10</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>77</v>
@@ -5500,15 +5689,15 @@
         <v>10</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>77</v>
@@ -5520,15 +5709,15 @@
         <v>10</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>77</v>
@@ -5540,15 +5729,15 @@
         <v>10</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>77</v>
@@ -5560,15 +5749,15 @@
         <v>10</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>77</v>
@@ -5580,15 +5769,15 @@
         <v>10</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>77</v>
@@ -5600,15 +5789,15 @@
         <v>10</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>77</v>
@@ -5620,15 +5809,15 @@
         <v>10</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>77</v>
@@ -5640,15 +5829,15 @@
         <v>10</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>77</v>
@@ -5660,15 +5849,15 @@
         <v>10</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>77</v>
@@ -5680,15 +5869,15 @@
         <v>10</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>77</v>
@@ -5700,15 +5889,15 @@
         <v>10</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>435</v>
+        <v>446</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>77</v>
@@ -5720,15 +5909,15 @@
         <v>10</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>77</v>
@@ -5740,15 +5929,15 @@
         <v>10</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>77</v>
@@ -5760,15 +5949,15 @@
         <v>10</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>77</v>
@@ -5780,15 +5969,15 @@
         <v>10</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>443</v>
+        <v>454</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>77</v>
@@ -5800,15 +5989,15 @@
         <v>10</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>77</v>
@@ -5820,15 +6009,15 @@
         <v>10</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>447</v>
+        <v>458</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>77</v>
@@ -5840,15 +6029,15 @@
         <v>10</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>77</v>
@@ -5860,15 +6049,15 @@
         <v>10</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>77</v>
@@ -5880,15 +6069,15 @@
         <v>10</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="58.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>77</v>
@@ -5900,15 +6089,15 @@
         <v>10</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>77</v>
@@ -5920,15 +6109,15 @@
         <v>10</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>77</v>
@@ -5940,15 +6129,15 @@
         <v>10</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>460</v>
+        <v>471</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>77</v>
@@ -5960,15 +6149,15 @@
         <v>10</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>77</v>
@@ -5980,15 +6169,15 @@
         <v>10</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>463</v>
+        <v>474</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>464</v>
+        <v>475</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>77</v>
@@ -6000,15 +6189,15 @@
         <v>10</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>465</v>
+        <v>476</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>466</v>
+        <v>477</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>77</v>
@@ -6020,15 +6209,15 @@
         <v>10</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>467</v>
+        <v>478</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>468</v>
+        <v>479</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>77</v>
@@ -6040,15 +6229,15 @@
         <v>10</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>470</v>
+        <v>481</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>77</v>
@@ -6060,15 +6249,15 @@
         <v>10</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>471</v>
+        <v>482</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>472</v>
+        <v>483</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>77</v>
@@ -6080,15 +6269,15 @@
         <v>10</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>77</v>
@@ -6100,15 +6289,15 @@
         <v>10</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>77</v>
@@ -6120,15 +6309,15 @@
         <v>10</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="B128" s="19" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>77</v>
@@ -6140,15 +6329,15 @@
         <v>10</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="B129" s="19" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>77</v>
@@ -6160,15 +6349,15 @@
         <v>10</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>482</v>
+        <v>493</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>77</v>
@@ -6180,15 +6369,15 @@
         <v>10</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>483</v>
+        <v>494</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>484</v>
+        <v>495</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>77</v>
@@ -6200,15 +6389,15 @@
         <v>10</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>486</v>
+        <v>497</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>77</v>
@@ -6220,15 +6409,15 @@
         <v>10</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>487</v>
+        <v>498</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>488</v>
+        <v>499</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>77</v>
@@ -6240,15 +6429,15 @@
         <v>10</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>77</v>
@@ -6260,15 +6449,15 @@
         <v>10</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>77</v>
@@ -6280,15 +6469,15 @@
         <v>10</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="B136" s="19" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>77</v>
@@ -6300,15 +6489,15 @@
         <v>10</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>495</v>
+        <v>506</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>77</v>
@@ -6320,15 +6509,15 @@
         <v>10</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>77</v>
@@ -6340,15 +6529,15 @@
         <v>10</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>500</v>
+        <v>511</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>77</v>
@@ -6360,15 +6549,15 @@
         <v>10</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="B140" s="19" t="s">
-        <v>502</v>
+        <v>513</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>77</v>
@@ -6380,15 +6569,15 @@
         <v>10</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>77</v>
@@ -6400,15 +6589,15 @@
         <v>10</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>505</v>
+        <v>516</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>77</v>
@@ -6420,15 +6609,15 @@
         <v>10</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>77</v>
@@ -6440,15 +6629,15 @@
         <v>10</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>77</v>
@@ -6460,15 +6649,15 @@
         <v>10</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>77</v>
@@ -6480,15 +6669,15 @@
         <v>10</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>77</v>
@@ -6500,15 +6689,15 @@
         <v>10</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>77</v>
@@ -6520,15 +6709,15 @@
         <v>10</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="B148" s="19" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>77</v>
@@ -6540,21 +6729,21 @@
         <v>10</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>519</v>
+        <v>530</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>520</v>
+        <v>531</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>10</v>
@@ -6565,6 +6754,18 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:H149">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="fDAI-6"/>
+        <filter val="fDOLA-6"/>
+        <filter val="fETH-6"/>
+        <filter val="fFEI-6"/>
+        <filter val="fUSDC-6"/>
+        <filter val="fsOHM-6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C90" r:id="rId1" display="https://etherscan.io/address/0x4ddc2d193948926d02f9b1fe9e1daa0718270ed5"/>
     <hyperlink ref="C91" r:id="rId2" display="https://etherscan.io/address/0xf650c3d88d12db855b8bf7d11be6c55a4e07dcc9"/>
@@ -6578,5 +6779,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add gauge contracts for DOLA3CRV
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="537">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -438,6 +438,12 @@
     <t xml:space="preserve">dolafraxbp_gauge</t>
   </si>
   <si>
+    <t xml:space="preserve">DOLA3CRV gauge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8Fa728F393588E8D8dD1ca397E9a710E53fA553a</t>
+  </si>
+  <si>
     <t xml:space="preserve">lending2</t>
   </si>
   <si>
@@ -474,6 +480,9 @@
     <t xml:space="preserve">Conversion</t>
   </si>
   <si>
+    <t xml:space="preserve">NewGaugeWeight </t>
+  </si>
+  <si>
     <t xml:space="preserve">NewBorrowCap</t>
   </si>
   <si>
@@ -493,6 +502,9 @@
   </si>
   <si>
     <t xml:space="preserve">Burn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VoteForGauge </t>
   </si>
   <si>
     <t xml:space="preserve">NewPriceOracle</t>
@@ -2115,7 +2127,7 @@
   <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3107,6 +3119,26 @@
         <v>10</v>
       </c>
       <c r="F49" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3142,7 +3174,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="1" sqref="D48 K14"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3166,10 +3198,10 @@
         <v>37</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>19</v>
@@ -3195,102 +3227,106 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="12"/>
+      <c r="L2" s="12" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="L3" s="12"/>
+        <v>155</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="L4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -3305,7 +3341,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -3321,7 +3357,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -3369,7 +3405,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="D48 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3393,16 +3429,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3467,7 +3503,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="D48 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3539,7 +3575,7 @@
   <dimension ref="A1:H150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A150" activeCellId="1" sqref="D48 A150"/>
+      <selection pane="topLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3556,19 +3592,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
@@ -3576,16 +3612,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>61</v>
@@ -3603,10 +3639,10 @@
         <v>80</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>77</v>
@@ -3618,19 +3654,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>175</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">IF(F4="",E4,G4)</f>
@@ -3639,19 +3675,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H5" s="0" t="str">
         <f aca="false">IF(F5="",E5,G5)</f>
@@ -3660,19 +3696,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>180</v>
       </c>
       <c r="H6" s="0" t="str">
         <f aca="false">IF(F6="",E6,G6)</f>
@@ -3681,19 +3717,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H7" s="0" t="str">
         <f aca="false">IF(F7="",E7,G7)</f>
@@ -3702,19 +3738,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H8" s="0" t="str">
         <f aca="false">IF(F8="",E8,G8)</f>
@@ -3723,19 +3759,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H9" s="0" t="str">
         <f aca="false">IF(F9="",E9,G9)</f>
@@ -3744,19 +3780,19 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H10" s="0" t="str">
         <f aca="false">IF(F10="",E10,G10)</f>
@@ -3765,19 +3801,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H11" s="0" t="str">
         <f aca="false">IF(F11="",E11,G11)</f>
@@ -3786,19 +3822,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">IF(F12="",E12,G12)</f>
@@ -3807,19 +3843,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H13" s="0" t="str">
         <f aca="false">IF(F13="",E13,G13)</f>
@@ -3828,19 +3864,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H14" s="0" t="str">
         <f aca="false">IF(F14="",E14,G14)</f>
@@ -3849,19 +3885,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">IF(F15="",E15,G15)</f>
@@ -3870,19 +3906,19 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">IF(F16="",E16,G16)</f>
@@ -3891,19 +3927,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="H17" s="0" t="str">
         <f aca="false">IF(F17="",E17,G17)</f>
@@ -3912,19 +3948,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>221</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>217</v>
       </c>
       <c r="H18" s="0" t="str">
         <f aca="false">IF(F18="",E18,G18)</f>
@@ -3939,10 +3975,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>36</v>
@@ -3954,19 +3990,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">IF(F20="",E20,G20)</f>
@@ -3975,19 +4011,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="H21" s="0" t="str">
         <f aca="false">IF(F21="",E21,G21)</f>
@@ -3996,19 +4032,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>231</v>
-      </c>
       <c r="E22" s="14" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">IF(F22="",E22,G22)</f>
@@ -4017,19 +4053,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H23" s="0" t="str">
         <f aca="false">IF(F23="",E23,G23)</f>
@@ -4038,19 +4074,19 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H24" s="0" t="str">
         <f aca="false">IF(F24="",E24,G24)</f>
@@ -4059,22 +4095,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4085,10 +4121,10 @@
         <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>106</v>
@@ -4105,10 +4141,10 @@
         <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>77</v>
@@ -4125,10 +4161,10 @@
         <v>17</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>18</v>
@@ -4145,16 +4181,16 @@
         <v>68</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,10 +4201,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>41</v>
@@ -4185,10 +4221,10 @@
         <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>41</v>
@@ -4205,10 +4241,10 @@
         <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>41</v>
@@ -4225,16 +4261,16 @@
         <v>48</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,10 +4281,10 @@
         <v>50</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>101</v>
@@ -4259,16 +4295,16 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>106</v>
@@ -4279,22 +4315,22 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4305,10 +4341,10 @@
         <v>12</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>13</v>
@@ -4319,594 +4355,594 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="F40" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>276</v>
-      </c>
       <c r="G40" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="G41" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>277</v>
-      </c>
       <c r="H41" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4917,10 +4953,10 @@
         <v>21</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>22</v>
@@ -4937,10 +4973,10 @@
         <v>21</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>22</v>
@@ -4951,152 +4987,152 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>69</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5107,16 +5143,16 @@
         <v>119</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>69</v>
@@ -5133,16 +5169,16 @@
         <v>122</v>
       </c>
       <c r="C70" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="F70" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>365</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>360</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>69</v>
@@ -5153,22 +5189,22 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>69</v>
@@ -5185,16 +5221,16 @@
         <v>124</v>
       </c>
       <c r="C72" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E72" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D72" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>365</v>
-      </c>
       <c r="F72" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>69</v>
@@ -5211,10 +5247,10 @@
         <v>27</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>18</v>
@@ -5231,10 +5267,10 @@
         <v>29</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>18</v>
@@ -5251,10 +5287,10 @@
         <v>31</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>18</v>
@@ -5271,10 +5307,10 @@
         <v>33</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>18</v>
@@ -5285,154 +5321,154 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>61</v>
@@ -5449,10 +5485,10 @@
         <v>60</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>61</v>
@@ -5469,10 +5505,10 @@
         <v>64</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>61</v>
@@ -5483,16 +5519,16 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E86" s="0" t="s">
         <v>61</v>
@@ -5503,16 +5539,16 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>61</v>
@@ -5523,16 +5559,16 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>61</v>
@@ -5543,16 +5579,16 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>61</v>
@@ -5563,82 +5599,82 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E92" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="E92" s="14" t="s">
-        <v>409</v>
-      </c>
       <c r="H92" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5646,18 +5682,18 @@
         <v>102</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>77</v>
@@ -5669,15 +5705,15 @@
         <v>10</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>77</v>
@@ -5689,15 +5725,15 @@
         <v>10</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>77</v>
@@ -5709,15 +5745,15 @@
         <v>10</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>77</v>
@@ -5729,15 +5765,15 @@
         <v>10</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>77</v>
@@ -5749,15 +5785,15 @@
         <v>10</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>77</v>
@@ -5769,15 +5805,15 @@
         <v>10</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>77</v>
@@ -5789,15 +5825,15 @@
         <v>10</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>77</v>
@@ -5809,15 +5845,15 @@
         <v>10</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>77</v>
@@ -5829,15 +5865,15 @@
         <v>10</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>77</v>
@@ -5849,15 +5885,15 @@
         <v>10</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>77</v>
@@ -5869,15 +5905,15 @@
         <v>10</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>77</v>
@@ -5889,15 +5925,15 @@
         <v>10</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>77</v>
@@ -5909,15 +5945,15 @@
         <v>10</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>77</v>
@@ -5929,15 +5965,15 @@
         <v>10</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>77</v>
@@ -5949,15 +5985,15 @@
         <v>10</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>77</v>
@@ -5969,15 +6005,15 @@
         <v>10</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>77</v>
@@ -5989,15 +6025,15 @@
         <v>10</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>77</v>
@@ -6009,15 +6045,15 @@
         <v>10</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>77</v>
@@ -6029,15 +6065,15 @@
         <v>10</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>77</v>
@@ -6049,15 +6085,15 @@
         <v>10</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>77</v>
@@ -6069,15 +6105,15 @@
         <v>10</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="58.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>77</v>
@@ -6089,15 +6125,15 @@
         <v>10</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>77</v>
@@ -6109,15 +6145,15 @@
         <v>10</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>77</v>
@@ -6129,15 +6165,15 @@
         <v>10</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>77</v>
@@ -6149,15 +6185,15 @@
         <v>10</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>77</v>
@@ -6169,15 +6205,15 @@
         <v>10</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>77</v>
@@ -6189,15 +6225,15 @@
         <v>10</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>77</v>
@@ -6209,15 +6245,15 @@
         <v>10</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>77</v>
@@ -6229,15 +6265,15 @@
         <v>10</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>77</v>
@@ -6249,15 +6285,15 @@
         <v>10</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>77</v>
@@ -6269,15 +6305,15 @@
         <v>10</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>77</v>
@@ -6289,15 +6325,15 @@
         <v>10</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>77</v>
@@ -6309,15 +6345,15 @@
         <v>10</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B128" s="19" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>77</v>
@@ -6329,15 +6365,15 @@
         <v>10</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B129" s="19" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>77</v>
@@ -6349,15 +6385,15 @@
         <v>10</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>77</v>
@@ -6369,15 +6405,15 @@
         <v>10</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>77</v>
@@ -6389,15 +6425,15 @@
         <v>10</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>77</v>
@@ -6409,15 +6445,15 @@
         <v>10</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>77</v>
@@ -6429,15 +6465,15 @@
         <v>10</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>77</v>
@@ -6449,15 +6485,15 @@
         <v>10</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>77</v>
@@ -6469,15 +6505,15 @@
         <v>10</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B136" s="19" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>77</v>
@@ -6489,15 +6525,15 @@
         <v>10</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>77</v>
@@ -6509,15 +6545,15 @@
         <v>10</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>77</v>
@@ -6529,15 +6565,15 @@
         <v>10</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>77</v>
@@ -6549,15 +6585,15 @@
         <v>10</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B140" s="19" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>77</v>
@@ -6569,15 +6605,15 @@
         <v>10</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>77</v>
@@ -6589,15 +6625,15 @@
         <v>10</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>77</v>
@@ -6609,15 +6645,15 @@
         <v>10</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>77</v>
@@ -6629,15 +6665,15 @@
         <v>10</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>77</v>
@@ -6649,15 +6685,15 @@
         <v>10</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>77</v>
@@ -6669,15 +6705,15 @@
         <v>10</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>77</v>
@@ -6689,15 +6725,15 @@
         <v>10</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>77</v>
@@ -6709,15 +6745,15 @@
         <v>10</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="46.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="B148" s="19" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>77</v>
@@ -6729,21 +6765,21 @@
         <v>10</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Fix OPT lag + minor things
</commit_message>
<xml_diff>
--- a/contracts.xlsx
+++ b/contracts.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="552">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -569,6 +569,9 @@
     <t xml:space="preserve">Burn</t>
   </si>
   <si>
+    <t xml:space="preserve">Repayment</t>
+  </si>
+  <si>
     <t xml:space="preserve">VoteForGauge </t>
   </si>
   <si>
@@ -582,6 +585,9 @@
   </si>
   <si>
     <t xml:space="preserve">RemoveLiquidityOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redemption</t>
   </si>
   <si>
     <t xml:space="preserve">NewSupplyCap</t>
@@ -2175,8 +2181,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D54" activeCellId="0" sqref="D54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3708,7 +3714,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3839,12 +3845,14 @@
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="K3" s="15" t="s">
+        <v>179</v>
+      </c>
       <c r="L3" s="15" t="s">
         <v>176</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15" t="s">
@@ -3853,17 +3861,17 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -3872,22 +3880,24 @@
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="K4" s="15" t="s">
+        <v>185</v>
+      </c>
       <c r="L4" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -3907,7 +3917,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -3928,7 +3938,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -4006,16 +4016,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4192,8 +4202,8 @@
   </sheetPr>
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4210,19 +4220,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -4230,16 +4240,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>63</v>
@@ -4257,10 +4267,10 @@
         <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>79</v>
@@ -4272,19 +4282,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>200</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H4" s="2" t="str">
         <f aca="false">IF(F4="",E4,G4)</f>
@@ -4293,19 +4303,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="H5" s="2" t="str">
         <f aca="false">IF(F5="",E5,G5)</f>
@@ -4314,19 +4324,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H6" s="2" t="str">
         <f aca="false">IF(F6="",E6,G6)</f>
@@ -4335,19 +4345,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H7" s="2" t="str">
         <f aca="false">IF(F7="",E7,G7)</f>
@@ -4356,19 +4366,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H8" s="2" t="str">
         <f aca="false">IF(F8="",E8,G8)</f>
@@ -4377,19 +4387,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H9" s="2" t="str">
         <f aca="false">IF(F9="",E9,G9)</f>
@@ -4398,19 +4408,19 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H10" s="2" t="str">
         <f aca="false">IF(F10="",E10,G10)</f>
@@ -4419,19 +4429,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H11" s="2" t="str">
         <f aca="false">IF(F11="",E11,G11)</f>
@@ -4440,19 +4450,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H12" s="2" t="str">
         <f aca="false">IF(F12="",E12,G12)</f>
@@ -4461,19 +4471,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H13" s="2" t="str">
         <f aca="false">IF(F13="",E13,G13)</f>
@@ -4482,19 +4492,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H14" s="2" t="str">
         <f aca="false">IF(F14="",E14,G14)</f>
@@ -4503,19 +4513,19 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H15" s="2" t="str">
         <f aca="false">IF(F15="",E15,G15)</f>
@@ -4524,19 +4534,19 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H16" s="2" t="str">
         <f aca="false">IF(F16="",E16,G16)</f>
@@ -4545,19 +4555,19 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="H17" s="2" t="str">
         <f aca="false">IF(F17="",E17,G17)</f>
@@ -4566,19 +4576,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H18" s="2" t="str">
         <f aca="false">IF(F18="",E18,G18)</f>
@@ -4593,10 +4603,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>38</v>
@@ -4608,19 +4618,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H20" s="2" t="str">
         <f aca="false">IF(F20="",E20,G20)</f>
@@ -4629,19 +4639,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H21" s="2" t="str">
         <f aca="false">IF(F21="",E21,G21)</f>
@@ -4650,19 +4660,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>256</v>
-      </c>
       <c r="E22" s="17" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="H22" s="2" t="str">
         <f aca="false">IF(F22="",E22,G22)</f>
@@ -4671,19 +4681,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H23" s="2" t="str">
         <f aca="false">IF(F23="",E23,G23)</f>
@@ -4692,19 +4702,19 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H24" s="2" t="str">
         <f aca="false">IF(F24="",E24,G24)</f>
@@ -4713,22 +4723,22 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4739,10 +4749,10 @@
         <v>107</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>108</v>
@@ -4759,10 +4769,10 @@
         <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>79</v>
@@ -4779,10 +4789,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>20</v>
@@ -4799,16 +4809,16 @@
         <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4819,10 +4829,10 @@
         <v>42</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>43</v>
@@ -4839,10 +4849,10 @@
         <v>46</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>43</v>
@@ -4859,10 +4869,10 @@
         <v>48</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>282</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>280</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>43</v>
@@ -4879,16 +4889,16 @@
         <v>50</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4899,10 +4909,10 @@
         <v>52</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>103</v>
@@ -4913,16 +4923,16 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>108</v>
@@ -4933,22 +4943,22 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4959,7 +4969,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>142</v>
@@ -4973,48 +4983,48 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5025,126 +5035,126 @@
         <v>148</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D40" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,100 +5165,100 @@
         <v>156</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5259,308 +5269,308 @@
         <v>152</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5571,10 +5581,10 @@
         <v>23</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>24</v>
@@ -5591,10 +5601,10 @@
         <v>23</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>24</v>
@@ -5611,146 +5621,146 @@
         <v>154</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5761,16 +5771,16 @@
         <v>121</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>71</v>
@@ -5787,16 +5797,16 @@
         <v>124</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>71</v>
@@ -5807,22 +5817,22 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>382</v>
-      </c>
       <c r="F71" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>71</v>
@@ -5839,16 +5849,16 @@
         <v>126</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>71</v>
@@ -5865,10 +5875,10 @@
         <v>29</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>20</v>
@@ -5885,10 +5895,10 @@
         <v>31</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>20</v>
@@ -5905,10 +5915,10 @@
         <v>33</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>20</v>
@@ -5925,10 +5935,10 @@
         <v>35</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>20</v>
@@ -5939,154 +5949,154 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="C79" s="2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>63</v>
@@ -6103,10 +6113,10 @@
         <v>62</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>63</v>
@@ -6123,10 +6133,10 @@
         <v>66</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>63</v>
@@ -6137,16 +6147,16 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>63</v>
@@ -6157,16 +6167,16 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>63</v>
@@ -6177,16 +6187,16 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>63</v>
@@ -6197,16 +6207,16 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>63</v>
@@ -6217,82 +6227,82 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="E91" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="E91" s="17" t="s">
-        <v>426</v>
-      </c>
       <c r="H91" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6300,18 +6310,18 @@
         <v>104</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C95" s="9" t="s">
         <v>79</v>
@@ -6323,15 +6333,15 @@
         <v>12</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C96" s="9" t="s">
         <v>79</v>
@@ -6343,15 +6353,15 @@
         <v>12</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C97" s="9" t="s">
         <v>79</v>
@@ -6363,15 +6373,15 @@
         <v>12</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C98" s="9" t="s">
         <v>79</v>
@@ -6383,15 +6393,15 @@
         <v>12</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>79</v>
@@ -6403,15 +6413,15 @@
         <v>12</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>79</v>
@@ -6423,15 +6433,15 @@
         <v>12</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>79</v>
@@ -6443,15 +6453,15 @@
         <v>12</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>79</v>
@@ -6463,15 +6473,15 @@
         <v>12</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>79</v>
@@ -6483,15 +6493,15 @@
         <v>12</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>79</v>
@@ -6503,15 +6513,15 @@
         <v>12</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>79</v>
@@ -6523,15 +6533,15 @@
         <v>12</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>79</v>
@@ -6543,15 +6553,15 @@
         <v>12</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>79</v>
@@ -6563,15 +6573,15 @@
         <v>12</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>79</v>
@@ -6583,15 +6593,15 @@
         <v>12</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>79</v>
@@ -6603,15 +6613,15 @@
         <v>12</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>79</v>
@@ -6623,15 +6633,15 @@
         <v>12</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>79</v>
@@ -6643,15 +6653,15 @@
         <v>12</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>79</v>
@@ -6663,15 +6673,15 @@
         <v>12</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>79</v>
@@ -6683,15 +6693,15 @@
         <v>12</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>79</v>
@@ -6703,15 +6713,15 @@
         <v>12</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C115" s="9" t="s">
         <v>79</v>
@@ -6723,15 +6733,15 @@
         <v>12</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>79</v>
@@ -6743,15 +6753,15 @@
         <v>12</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C117" s="9" t="s">
         <v>79</v>
@@ -6763,15 +6773,15 @@
         <v>12</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C118" s="9" t="s">
         <v>79</v>
@@ -6783,15 +6793,15 @@
         <v>12</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C119" s="9" t="s">
         <v>79</v>
@@ -6803,15 +6813,15 @@
         <v>12</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C120" s="9" t="s">
         <v>79</v>
@@ -6823,15 +6833,15 @@
         <v>12</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>79</v>
@@ -6843,15 +6853,15 @@
         <v>12</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C122" s="9" t="s">
         <v>79</v>
@@ -6863,15 +6873,15 @@
         <v>12</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C123" s="9" t="s">
         <v>79</v>
@@ -6883,15 +6893,15 @@
         <v>12</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C124" s="9" t="s">
         <v>79</v>
@@ -6903,15 +6913,15 @@
         <v>12</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C125" s="9" t="s">
         <v>79</v>
@@ -6923,15 +6933,15 @@
         <v>12</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>79</v>
@@ -6943,15 +6953,15 @@
         <v>12</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>79</v>
@@ -6963,15 +6973,15 @@
         <v>12</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>79</v>
@@ -6983,15 +6993,15 @@
         <v>12</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>79</v>
@@ -7003,15 +7013,15 @@
         <v>12</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>79</v>
@@ -7023,15 +7033,15 @@
         <v>12</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>79</v>
@@ -7043,15 +7053,15 @@
         <v>12</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>79</v>
@@ -7063,15 +7073,15 @@
         <v>12</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C133" s="9" t="s">
         <v>79</v>
@@ -7083,15 +7093,15 @@
         <v>12</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C134" s="9" t="s">
         <v>79</v>
@@ -7103,15 +7113,15 @@
         <v>12</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C135" s="9" t="s">
         <v>79</v>
@@ -7123,15 +7133,15 @@
         <v>12</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>79</v>
@@ -7143,15 +7153,15 @@
         <v>12</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>79</v>
@@ -7163,15 +7173,15 @@
         <v>12</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C138" s="9" t="s">
         <v>79</v>
@@ -7183,15 +7193,15 @@
         <v>12</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>79</v>
@@ -7203,15 +7213,15 @@
         <v>12</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>79</v>
@@ -7223,15 +7233,15 @@
         <v>12</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C141" s="9" t="s">
         <v>79</v>
@@ -7243,15 +7253,15 @@
         <v>12</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C142" s="9" t="s">
         <v>79</v>
@@ -7263,15 +7273,15 @@
         <v>12</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C143" s="9" t="s">
         <v>79</v>
@@ -7283,15 +7293,15 @@
         <v>12</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C144" s="9" t="s">
         <v>79</v>
@@ -7303,15 +7313,15 @@
         <v>12</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C145" s="9" t="s">
         <v>79</v>
@@ -7323,15 +7333,15 @@
         <v>12</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C146" s="9" t="s">
         <v>79</v>
@@ -7343,15 +7353,15 @@
         <v>12</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C147" s="9" t="s">
         <v>79</v>
@@ -7363,15 +7373,15 @@
         <v>12</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C148" s="9" t="s">
         <v>79</v>
@@ -7383,21 +7393,21 @@
         <v>12</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>12</v>

</xml_diff>